<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@fa0becf77209d5cf83125339f2ba263d2c88d564 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="415">
   <si>
     <t>Row</t>
   </si>
@@ -106,10 +106,10 @@
     <t>1nF</t>
   </si>
   <si>
-    <t>C_Disc_D7.5mm_W4.4mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>Capacitor_THT</t>
+    <t>C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD</t>
   </si>
   <si>
     <t>2</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C322C101K1G5TA7301.pdf</t>
+    <t>http://www.holystonecaps.com/PDF/201612051329150.2017%20HVC%20Series.pdf</t>
   </si>
   <si>
     <t>/Power Supply</t>
@@ -157,13 +157,13 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C_Disc_D3.0mm_W1.6mm_P2.50mm</t>
+    <t>C_0805_2012Metric</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>https://www.vishay.com/docs/45171/kseries.pdf</t>
+    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
   </si>
   <si>
     <t>/MIDI</t>
@@ -187,16 +187,16 @@
     <t>3</t>
   </si>
   <si>
-    <t>C16 C17</t>
+    <t>C16 C17 C20</t>
   </si>
   <si>
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C_Disc_D5.1mm_W3.2mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C322C102K1R5TA.pdf</t>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(3)</t>
   </si>
   <si>
     <t>138.6376</t>
@@ -217,16 +217,13 @@
     <t>C13 C14 C15</t>
   </si>
   <si>
-    <t>220uF</t>
-  </si>
-  <si>
-    <t>CP_Radial_D10.0mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>https://www.cde.com/resources/catalogs/AVG.pdf</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(3)</t>
+    <t>270uF</t>
+  </si>
+  <si>
+    <t>CP_Elec_10x10</t>
+  </si>
+  <si>
+    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/A768MS277M1GLAE022</t>
   </si>
   <si>
     <t>140.5323</t>
@@ -244,6 +241,45 @@
     <t>5</t>
   </si>
   <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4</t>
+  </si>
+  <si>
+    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>LED_SMD</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+  </si>
+  <si>
+    <t>/LEDs</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(4)</t>
+  </si>
+  <si>
+    <t>45.6000</t>
+  </si>
+  <si>
+    <t>77.0000</t>
+  </si>
+  <si>
+    <t>4.8100</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>100V 0.15A standard switching diode, DO-35</t>
   </si>
   <si>
@@ -256,13 +292,16 @@
     <t>D11</t>
   </si>
   <si>
-    <t>D_DO-35_SOD27_P7.62mm_Horizontal</t>
-  </si>
-  <si>
-    <t>Diode_THT</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/download/data-sheet/pdf/1n914-d.pdf</t>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>Diode_SMD</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
   </si>
   <si>
     <t>pedalboard-hw(1)</t>
@@ -280,36 +319,6 @@
     <t>9.2200</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>100V 3A General Purpose Rectifier Diode, DO-201AD</t>
-  </si>
-  <si>
-    <t>1N5401</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>D_DO-201AD_P15.24mm_Horizontal</t>
-  </si>
-  <si>
-    <t>http://www.vishay.com/docs/88516/1n5400.pdf</t>
-  </si>
-  <si>
-    <t>134.7000</t>
-  </si>
-  <si>
-    <t>79.1000</t>
-  </si>
-  <si>
-    <t>18.4400</t>
-  </si>
-  <si>
-    <t>3.2000</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -322,10 +331,13 @@
     <t>D13</t>
   </si>
   <si>
-    <t>D_DO-41_SOD81_P10.16mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/1n5817-d.pdf</t>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
   </si>
   <si>
     <t>129.6060</t>
@@ -346,144 +358,111 @@
     <t>8</t>
   </si>
   <si>
-    <t>RGB LED with integrated controller, 5mm/8mm LED package</t>
-  </si>
-  <si>
-    <t>NeoPixel_THT</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4</t>
-  </si>
-  <si>
-    <t>NEOPIX</t>
-  </si>
-  <si>
-    <t>LED_D5.0mm-NeoPixel</t>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>151.9000</t>
+  </si>
+  <si>
+    <t>95.2000</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Fuse, small symbol</t>
+  </si>
+  <si>
+    <t>Fuse_Small</t>
+  </si>
+  <si>
+    <t>F2 F3 F4 F5</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Trace_Fuse</t>
   </si>
   <si>
     <t>Pedalboard Library</t>
   </si>
   <si>
-    <t>https://cdn.sparkfun.com/assets/6/9/0/f/3/DS-12999-LED_-_RGB_Addressable__PTH__5mm_Clear__5_Pack_.pdf</t>
-  </si>
-  <si>
-    <t>/LEDs</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(4)</t>
-  </si>
-  <si>
-    <t>45.6000</t>
-  </si>
-  <si>
-    <t>77.0000</t>
-  </si>
-  <si>
-    <t>4.8100</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/1n5400-d.pdf</t>
-  </si>
-  <si>
-    <t>151.9000</t>
-  </si>
-  <si>
-    <t>95.2000</t>
+    <t>66.9900</t>
+  </si>
+  <si>
+    <t>50.3100</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>4.8860</t>
+  </si>
+  <si>
+    <t>1.5240</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>Fuse, small symbol</t>
-  </si>
-  <si>
-    <t>Fuse_Small</t>
-  </si>
-  <si>
-    <t>F2 F3 F4 F5</t>
-  </si>
-  <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>Trace_Fuse</t>
-  </si>
-  <si>
-    <t>66.9900</t>
-  </si>
-  <si>
-    <t>50.3100</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>4.8860</t>
-  </si>
-  <si>
-    <t>1.5240</t>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>159.4000</t>
+  </si>
+  <si>
+    <t>94.6000</t>
+  </si>
+  <si>
+    <t>7.9000</t>
+  </si>
+  <si>
+    <t>7.6000</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>159.4000</t>
-  </si>
-  <si>
-    <t>94.6000</t>
-  </si>
-  <si>
-    <t>7.9000</t>
-  </si>
-  <si>
-    <t>7.6000</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -517,397 +496,412 @@
     <t>4.2400</t>
   </si>
   <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>J3 J9 J10 J11 J12</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(5)</t>
+  </si>
+  <si>
+    <t>155.6150</t>
+  </si>
+  <si>
+    <t>91.2000</t>
+  </si>
+  <si>
+    <t>15.7000</t>
+  </si>
+  <si>
+    <t>19.2300</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>J3 J9 J10 J11 J12</t>
-  </si>
-  <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(5)</t>
-  </si>
-  <si>
-    <t>155.6150</t>
-  </si>
-  <si>
-    <t>91.2000</t>
-  </si>
-  <si>
-    <t>15.7000</t>
-  </si>
-  <si>
-    <t>19.2300</t>
+    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Raspberry_Pi_2_3</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>HiFi Berry</t>
+  </si>
+  <si>
+    <t>HiFi Berry DAC ADC+</t>
+  </si>
+  <si>
+    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
+  </si>
+  <si>
+    <t>/Audio</t>
+  </si>
+  <si>
+    <t>100.2500</t>
+  </si>
+  <si>
+    <t>56.6244</t>
+  </si>
+  <si>
+    <t>41.4500</t>
+  </si>
+  <si>
+    <t>55.0150</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
-  </si>
-  <si>
-    <t>Raspberry_Pi_2_3</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>HiFi Berry</t>
-  </si>
-  <si>
-    <t>HiFi Berry DAC ADC+</t>
-  </si>
-  <si>
-    <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
-  </si>
-  <si>
-    <t>/Audio</t>
-  </si>
-  <si>
-    <t>100.2500</t>
-  </si>
-  <si>
-    <t>56.6244</t>
-  </si>
-  <si>
-    <t>41.4500</t>
-  </si>
-  <si>
-    <t>55.0150</t>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>J18 J19 J20 J21 J22 J23</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(6)</t>
+  </si>
+  <si>
+    <t>149.0000</t>
+  </si>
+  <si>
+    <t>57.0000</t>
+  </si>
+  <si>
+    <t>3.3500</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>J18 J19 J20 J21 J22 J23</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(6)</t>
-  </si>
-  <si>
-    <t>149.0000</t>
-  </si>
-  <si>
-    <t>57.0000</t>
-  </si>
-  <si>
-    <t>3.3500</t>
+    <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Top_Bottom</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>MIDI IN/OUT</t>
+  </si>
+  <si>
+    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx21021.pdf</t>
+  </si>
+  <si>
+    <t>51.0000</t>
+  </si>
+  <si>
+    <t>72.1500</t>
+  </si>
+  <si>
+    <t>6.7800</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x03, top/bottom pin numbering scheme (row 1: 1...pins_per_row, row2: pins_per_row+1 ... num_pins), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Top_Bottom</t>
-  </si>
-  <si>
-    <t>J15</t>
-  </si>
-  <si>
-    <t>MIDI IN/OUT</t>
-  </si>
-  <si>
-    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx21021.pdf</t>
-  </si>
-  <si>
-    <t>51.0000</t>
-  </si>
-  <si>
-    <t>72.1500</t>
-  </si>
-  <si>
-    <t>6.7800</t>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J16 J17</t>
+  </si>
+  <si>
+    <t>MIDI OUT J</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>96.0000</t>
+  </si>
+  <si>
+    <t>100.5000</t>
+  </si>
+  <si>
+    <t>11.2000</t>
+  </si>
+  <si>
+    <t>6.7000</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J16 J17</t>
-  </si>
-  <si>
-    <t>MIDI OUT J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>96.0000</t>
-  </si>
-  <si>
-    <t>100.5000</t>
-  </si>
-  <si>
-    <t>11.2000</t>
-  </si>
-  <si>
-    <t>6.7000</t>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>MIDI_OUT</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>103.0000</t>
+  </si>
+  <si>
+    <t>17.5000</t>
+  </si>
+  <si>
+    <t>14.7500</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
-  </si>
-  <si>
-    <t>MIDI_OUT</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>103.0000</t>
-  </si>
-  <si>
-    <t>17.5000</t>
-  </si>
-  <si>
-    <t>14.7500</t>
+    <t>Generic connector, single row, 01x02, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x02_Pin</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Pico USB TP</t>
+  </si>
+  <si>
+    <t>Spring_Loaded_Pins_2mm</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
+  </si>
+  <si>
+    <t>107.0000</t>
+  </si>
+  <si>
+    <t>1.3500</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x02, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Pico USB TP</t>
-  </si>
-  <si>
-    <t>Spring_Loaded_Pins_2mm</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
-  </si>
-  <si>
-    <t>107.0000</t>
-  </si>
-  <si>
-    <t>1.3500</t>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
+  </si>
+  <si>
+    <t>35.8650</t>
+  </si>
+  <si>
+    <t>42.0374</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
-  </si>
-  <si>
-    <t>35.8650</t>
-  </si>
-  <si>
-    <t>42.0374</t>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Raspberry_pi</t>
+  </si>
+  <si>
+    <t>Raspberry PI Compute Module CM4 Nano A</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
+  </si>
+  <si>
+    <t>29.5900</t>
+  </si>
+  <si>
+    <t>18.6800</t>
+  </si>
+  <si>
+    <t>49.9600</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Raspberry_pi</t>
-  </si>
-  <si>
-    <t>Raspberry PI Compute Module CM4 Nano A</t>
-  </si>
-  <si>
-    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
-  </si>
-  <si>
-    <t>29.5900</t>
-  </si>
-  <si>
-    <t>18.6800</t>
-  </si>
-  <si>
-    <t>49.9600</t>
+    <t>USB Type A connector</t>
+  </si>
+  <si>
+    <t>USB_A</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>USB A BCB Male Plug</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
+  </si>
+  <si>
+    <t>93.6250</t>
+  </si>
+  <si>
+    <t>27.2200</t>
+  </si>
+  <si>
+    <t>9.3200</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>USB Type A connector</t>
-  </si>
-  <si>
-    <t>USB_A</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>USB A BCB Male Plug</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
-  </si>
-  <si>
-    <t>93.6250</t>
-  </si>
-  <si>
-    <t>27.2200</t>
-  </si>
-  <si>
-    <t>9.3200</t>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>L_1210_3225Metric</t>
+  </si>
+  <si>
+    <t>Inductor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
+  </si>
+  <si>
+    <t>141.9000</t>
+  </si>
+  <si>
+    <t>74.7000</t>
+  </si>
+  <si>
+    <t>2.6000</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>L_Radial_D12.0mm_P5.00mm_Fastron_11P</t>
-  </si>
-  <si>
-    <t>Inductor_THT</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Wurth%20Electronics%20PDFs/7447471022.pdf</t>
-  </si>
-  <si>
-    <t>141.9000</t>
-  </si>
-  <si>
-    <t>74.7000</t>
-  </si>
-  <si>
-    <t>2.6000</t>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4 L5</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>56.6000</t>
+  </si>
+  <si>
+    <t>69.7300</t>
+  </si>
+  <si>
+    <t>11.7600</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4 L5</t>
-  </si>
-  <si>
-    <t>103_100MHz</t>
-  </si>
-  <si>
-    <t>L_Axial_L6.6mm_D2.7mm_P10.16mm_Horizontal_Vishay_IM-2</t>
-  </si>
-  <si>
-    <t>https://www.fair-rite.com/wp-content/themes/fair-rite/print_product.php?pid=18584</t>
-  </si>
-  <si>
-    <t>56.6000</t>
-  </si>
-  <si>
-    <t>69.7300</t>
-  </si>
-  <si>
-    <t>11.7600</t>
+    <t/>
+  </si>
+  <si>
+    <t>PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
+  </si>
+  <si>
+    <t>114.8000</t>
+  </si>
+  <si>
+    <t>43.3200</t>
+  </si>
+  <si>
+    <t>22.5700</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>PS1</t>
-  </si>
-  <si>
-    <t>CONV_PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
-  </si>
-  <si>
-    <t>114.8000</t>
-  </si>
-  <si>
-    <t>43.3200</t>
-  </si>
-  <si>
-    <t>22.5700</t>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>-20.0000</t>
+  </si>
+  <si>
+    <t>125.0000</t>
   </si>
   <si>
     <t>26</t>
@@ -922,13 +916,13 @@
     <t>R4</t>
   </si>
   <si>
-    <t>R_Axial_DIN0207_L6.3mm_D2.5mm_P10.16mm_Horizontal</t>
-  </si>
-  <si>
-    <t>Resistor_THT</t>
-  </si>
-  <si>
-    <t>https://www.koaspeer.com/pdfs/CF.pdf</t>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>Resistor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
   </si>
   <si>
     <t>61.1900</t>
@@ -946,6 +940,9 @@
     <t>33</t>
   </si>
   <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
     <t>27.6950</t>
   </si>
   <si>
@@ -955,7 +952,7 @@
     <t>28</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1 R5</t>
   </si>
   <si>
     <t>220</t>
@@ -970,72 +967,66 @@
     <t>29</t>
   </si>
   <si>
-    <t>R2 R5</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>58.9500</t>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SW_SPST_B3S-1000</t>
+  </si>
+  <si>
+    <t>Button_Switch_SMD</t>
+  </si>
+  <si>
+    <t>https://omronfs.omron.com/en_US/ecb/products/pdf/en-b3s.pdf</t>
+  </si>
+  <si>
+    <t>3.7500</t>
+  </si>
+  <si>
+    <t>8.5000</t>
+  </si>
+  <si>
+    <t>15.5000</t>
+  </si>
+  <si>
+    <t>7.5000</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth-430476085716</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430466043726.pdf</t>
-  </si>
-  <si>
-    <t>3.7500</t>
-  </si>
-  <si>
-    <t>8.5000</t>
-  </si>
-  <si>
-    <t>15.5000</t>
-  </si>
-  <si>
-    <t>7.5000</t>
+    <t>SW5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>78.7500</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>78.7500</t>
+    <t>SW6</t>
+  </si>
+  <si>
+    <t>153.7500</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>SW6</t>
-  </si>
-  <si>
-    <t>153.7500</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -1045,103 +1036,124 @@
     <t>60.5000</t>
   </si>
   <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>E</t>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>GAIN Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>115.2500</t>
+  </si>
+  <si>
+    <t>93.5000</t>
+  </si>
+  <si>
+    <t>16.5000</t>
+  </si>
+  <si>
+    <t>14.4000</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>115.2500</t>
-  </si>
-  <si>
-    <t>93.5000</t>
-  </si>
-  <si>
-    <t>16.5000</t>
-  </si>
-  <si>
-    <t>14.4000</t>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>VOL Rotary</t>
+  </si>
+  <si>
+    <t>40.2500</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
-  </si>
-  <si>
-    <t>40.2500</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOT65P210X110-5N</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>52.9500</t>
+  </si>
+  <si>
+    <t>77.9500</t>
+  </si>
+  <si>
+    <t>2.5500</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>OR Gate IC 1 Channel - SOT-353</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD</t>
-  </si>
-  <si>
-    <t>52.9500</t>
-  </si>
-  <si>
-    <t>77.9500</t>
-  </si>
-  <si>
-    <t>2.5500</t>
+    <t>Pico</t>
+  </si>
+  <si>
+    <t>MCU_RaspberryPi_and_Boards</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>RPi_Pico_SMD_TH</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
+  </si>
+  <si>
+    <t>83.0000</t>
+  </si>
+  <si>
+    <t>76.0000</t>
+  </si>
+  <si>
+    <t>19.4800</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>Schmitt Trigger Output Optocoupler, High Speed, DIP-6, 1.6mA turn on threshold</t>
-  </si>
-  <si>
-    <t>H11L1</t>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
   </si>
   <si>
     <t>Isolator</t>
@@ -1150,13 +1162,13 @@
     <t>U2</t>
   </si>
   <si>
-    <t>DIP-6_W7.62mm_LongPads</t>
-  </si>
-  <si>
-    <t>Package_DIP</t>
-  </si>
-  <si>
-    <t>https://rocelec.widen.net/view/pdf/rwjc9al1ln/ONSM-S-A0003590761-1.pdf</t>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Package_SO</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
   </si>
   <si>
     <t>49.4750</t>
@@ -1171,33 +1183,6 @@
     <t>6.6800</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Pico</t>
-  </si>
-  <si>
-    <t>MCU_RaspberryPi_and_Boards</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
-  </si>
-  <si>
-    <t>83.0000</t>
-  </si>
-  <si>
-    <t>76.0000</t>
-  </si>
-  <si>
-    <t>19.4800</t>
-  </si>
-  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -1237,13 +1222,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>83 (5 SMD/ 76 THT)</t>
+    <t>83 (5 SMD/ 75 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>77 (5 SMD/ 70 THT)</t>
+    <t>77 (5 SMD/ 69 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1369,13 +1354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1828,7 +1813,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1863,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1887,55 +1872,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F2" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1943,13 +1928,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F6" s="3">
         <v>77</v>
@@ -2179,28 +2164,28 @@
         <v>56</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>59</v>
@@ -2227,7 +2212,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>61</v>
       </c>
@@ -2268,13 +2253,13 @@
         <v>33</v>
       </c>
       <c r="N12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="P12" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="Q12" s="10" t="s">
         <v>52</v>
@@ -2289,51 +2274,51 @@
         <v>40</v>
       </c>
       <c r="U12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="V12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="V12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:22" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="N13" s="5" t="s">
         <v>81</v>
@@ -2345,7 +2330,7 @@
         <v>83</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>38</v>
@@ -2357,36 +2342,36 @@
         <v>40</v>
       </c>
       <c r="U13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="30" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="V13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>88</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>89</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>22</v>
@@ -2398,22 +2383,22 @@
         <v>31</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>
@@ -2425,36 +2410,36 @@
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>22</v>
@@ -2466,22 +2451,22 @@
         <v>31</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>38</v>
@@ -2493,63 +2478,63 @@
         <v>40</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>38</v>
@@ -2561,10 +2546,10 @@
         <v>40</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -2583,29 +2568,29 @@
       <c r="E17" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="11" t="s">
         <v>125</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>127</v>
+      <c r="L17" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>81</v>
@@ -2617,116 +2602,116 @@
         <v>129</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="R17" s="7" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>134</v>
+      <c r="L18" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="T18" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="30" customHeight="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="60" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>22</v>
@@ -2738,25 +2723,25 @@
         <v>31</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="M19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="R19" s="7" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S19" s="7" t="s">
         <v>39</v>
@@ -2765,66 +2750,66 @@
         <v>40</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="60" customHeight="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S20" s="10" t="s">
         <v>39</v>
@@ -2833,66 +2818,66 @@
         <v>40</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="V20" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S21" s="7" t="s">
         <v>39</v>
@@ -2901,66 +2886,66 @@
         <v>40</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="30" customHeight="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="45" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L22" s="10" t="s">
-        <v>184</v>
+      <c r="L22" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>185</v>
+        <v>80</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S22" s="10" t="s">
         <v>39</v>
@@ -2969,66 +2954,66 @@
         <v>40</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="45" customHeight="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="60" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="12" t="s">
-        <v>134</v>
+      <c r="L23" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>196</v>
+        <v>94</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S23" s="7" t="s">
         <v>39</v>
@@ -3037,66 +3022,66 @@
         <v>40</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>199</v>
+        <v>157</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="60" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="30" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M24" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="Q24" s="10" t="s">
         <v>37</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S24" s="10" t="s">
         <v>39</v>
@@ -3105,36 +3090,36 @@
         <v>40</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="30" customHeight="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="5" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>30</v>
@@ -3146,7 +3131,7 @@
         <v>31</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>48</v>
@@ -3155,10 +3140,10 @@
         <v>34</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="Q25" s="7" t="s">
         <v>37</v>
@@ -3167,110 +3152,110 @@
         <v>38</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="M26" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>228</v>
+        <v>83</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>37</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="T26" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>22</v>
@@ -3282,25 +3267,25 @@
         <v>31</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>119</v>
+        <v>240</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="R27" s="7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="S27" s="7" t="s">
         <v>39</v>
@@ -3309,36 +3294,36 @@
         <v>40</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="30" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="G28" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>245</v>
-      </c>
       <c r="H28" s="10" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>22</v>
@@ -3350,25 +3335,25 @@
         <v>31</v>
       </c>
       <c r="L28" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O28" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="M28" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="O28" s="10" t="s">
+      <c r="P28" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="P28" s="10" t="s">
-        <v>248</v>
-      </c>
       <c r="Q28" s="10" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S28" s="10" t="s">
         <v>39</v>
@@ -3377,36 +3362,36 @@
         <v>40</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="V28" s="10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>249</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>180</v>
+        <v>251</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>251</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>22</v>
@@ -3418,25 +3403,25 @@
         <v>31</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S29" s="7" t="s">
         <v>39</v>
@@ -3445,36 +3430,36 @@
         <v>40</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="30" customHeight="1">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>114</v>
+        <v>264</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>22</v>
@@ -3486,25 +3471,25 @@
         <v>31</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>185</v>
+        <v>33</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="R30" s="10" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="S30" s="10" t="s">
         <v>39</v>
@@ -3513,63 +3498,63 @@
         <v>40</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="V30" s="10" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>81</v>
+        <v>165</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>38</v>
@@ -3581,63 +3566,63 @@
         <v>40</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="30" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>25</v>
+        <v>281</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>281</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>272</v>
+        <v>127</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="K32" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>173</v>
+        <v>94</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="R32" s="10" t="s">
         <v>38</v>
@@ -3649,18 +3634,18 @@
         <v>40</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="V32" s="10" t="s">
-        <v>42</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B33" s="12" t="s">
         <v>288</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>289</v>
@@ -3678,7 +3663,7 @@
         <v>291</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>22</v>
@@ -3689,64 +3674,64 @@
       <c r="K33" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>292</v>
+      <c r="L33" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O33" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="P33" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="P33" s="7" t="s">
-        <v>294</v>
-      </c>
       <c r="Q33" s="7" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="T33" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>295</v>
+        <v>52</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>295</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>298</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H34" s="10" t="s">
         <v>299</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>301</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>22</v>
@@ -3758,19 +3743,19 @@
         <v>31</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>52</v>
@@ -3785,7 +3770,7 @@
         <v>40</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="V34" s="10" t="s">
         <v>42</v>
@@ -3793,28 +3778,28 @@
     </row>
     <row r="35" spans="1:22">
       <c r="A35" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>22</v>
@@ -3826,19 +3811,19 @@
         <v>31</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O35" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="P35" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="P35" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="Q35" s="7" t="s">
         <v>52</v>
@@ -3853,7 +3838,7 @@
         <v>40</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>42</v>
@@ -3861,52 +3846,52 @@
     </row>
     <row r="36" spans="1:22">
       <c r="A36" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>312</v>
-      </c>
       <c r="G36" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="M36" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="O36" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="P36" s="10" t="s">
         <v>313</v>
-      </c>
-      <c r="P36" s="10" t="s">
-        <v>314</v>
       </c>
       <c r="Q36" s="10" t="s">
         <v>37</v>
@@ -3921,7 +3906,7 @@
         <v>40</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="V36" s="10" t="s">
         <v>42</v>
@@ -3929,52 +3914,52 @@
     </row>
     <row r="37" spans="1:22">
       <c r="A37" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>297</v>
-      </c>
       <c r="C37" s="7" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>25</v>
+        <v>317</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="M37" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="P37" s="7" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="Q37" s="7" t="s">
         <v>52</v>
@@ -3989,36 +3974,36 @@
         <v>40</v>
       </c>
       <c r="U37" s="7" t="s">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="8" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="G38" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="H38" s="10" t="s">
         <v>321</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>22</v>
@@ -4030,19 +4015,19 @@
         <v>31</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M38" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="Q38" s="10" t="s">
         <v>52</v>
@@ -4057,36 +4042,36 @@
         <v>40</v>
       </c>
       <c r="U38" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="V38" s="10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="5" t="s">
         <v>331</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>332</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>333</v>
+        <v>24</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>114</v>
+        <v>321</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>22</v>
@@ -4098,19 +4083,19 @@
         <v>31</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M39" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="Q39" s="7" t="s">
         <v>52</v>
@@ -4125,36 +4110,36 @@
         <v>40</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="F40" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="H40" s="10" t="s">
         <v>321</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>22</v>
@@ -4166,19 +4151,19 @@
         <v>31</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M40" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O40" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="P40" s="10" t="s">
         <v>337</v>
-      </c>
-      <c r="P40" s="10" t="s">
-        <v>328</v>
       </c>
       <c r="Q40" s="10" t="s">
         <v>52</v>
@@ -4193,24 +4178,24 @@
         <v>40</v>
       </c>
       <c r="U40" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="V40" s="10" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>338</v>
@@ -4219,10 +4204,10 @@
         <v>339</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>114</v>
+        <v>321</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>22</v>
@@ -4234,19 +4219,19 @@
         <v>31</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M41" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O41" s="7" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="P41" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Q41" s="7" t="s">
         <v>52</v>
@@ -4261,36 +4246,36 @@
         <v>40</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="30" customHeight="1">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="F42" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="H42" s="10" t="s">
         <v>321</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>22</v>
@@ -4302,19 +4287,19 @@
         <v>31</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="M42" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Q42" s="10" t="s">
         <v>52</v>
@@ -4329,36 +4314,36 @@
         <v>40</v>
       </c>
       <c r="U42" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="V42" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>320</v>
-      </c>
       <c r="C43" s="7" t="s">
-        <v>321</v>
+        <v>345</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>322</v>
+        <v>25</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>22</v>
@@ -4370,19 +4355,19 @@
         <v>31</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="M43" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="Q43" s="7" t="s">
         <v>52</v>
@@ -4397,36 +4382,36 @@
         <v>40</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>22</v>
@@ -4438,19 +4423,19 @@
         <v>31</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="M44" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O44" s="10" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Q44" s="10" t="s">
         <v>52</v>
@@ -4465,36 +4450,36 @@
         <v>40</v>
       </c>
       <c r="U44" s="10" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="V44" s="10" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="30" customHeight="1">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>348</v>
+      <c r="B45" s="11" t="s">
+        <v>280</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>25</v>
+        <v>359</v>
       </c>
       <c r="E45" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>360</v>
-      </c>
       <c r="G45" s="7" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>22</v>
@@ -4506,63 +4491,63 @@
         <v>31</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O45" s="7" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="T45" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U45" s="7" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>363</v>
+        <v>366</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>280</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>367</v>
+        <v>127</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>22</v>
@@ -4573,64 +4558,64 @@
       <c r="K46" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L46" s="11" t="s">
-        <v>288</v>
+      <c r="L46" s="10" t="s">
+        <v>371</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O46" s="10" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="Q46" s="10" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="S46" s="10" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="T46" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U46" s="10" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="V46" s="10" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>22</v>
@@ -4642,19 +4627,19 @@
         <v>31</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="P47" s="7" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="Q47" s="7" t="s">
         <v>37</v>
@@ -4669,78 +4654,10 @@
         <v>40</v>
       </c>
       <c r="U47" s="7" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" ht="30" customHeight="1">
-      <c r="A48" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="E48" s="10" t="s">
         <v>386</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L48" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="M48" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N48" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="O48" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="P48" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="Q48" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="R48" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="S48" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="T48" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="U48" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="V48" s="10" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4765,12 +4682,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" customWidth="1"/>
@@ -4790,7 +4707,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4814,55 +4731,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F2" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4870,13 +4787,13 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F6" s="3">
         <v>77</v>
@@ -4955,49 +4872,49 @@
         <v>22</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>52</v>
@@ -5009,13 +4926,13 @@
         <v>39</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -5041,22 +4958,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="12" t="s">
-        <v>419</v>
+      <c r="A4" s="11" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@c8098e8a46af51d98cde4a1485d4c95c69d75496 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -566,181 +566,181 @@
     <t>~</t>
   </si>
   <si>
-    <t>149.0000</t>
-  </si>
-  <si>
-    <t>57.0000</t>
+    <t>159.0000</t>
+  </si>
+  <si>
+    <t>69.0000</t>
+  </si>
+  <si>
+    <t>3.3500</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Odd_Even</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>MIDI IN/OUT</t>
+  </si>
+  <si>
+    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>24.8500</t>
+  </si>
+  <si>
+    <t>80.0750</t>
+  </si>
+  <si>
+    <t>6.7800</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J16 J17</t>
+  </si>
+  <si>
+    <t>MIDI OUT J</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>96.0000</t>
+  </si>
+  <si>
+    <t>100.5000</t>
+  </si>
+  <si>
+    <t>11.2000</t>
+  </si>
+  <si>
+    <t>6.7000</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J1 J2</t>
+  </si>
+  <si>
+    <t>MIDI_OUT</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>103.0000</t>
+  </si>
+  <si>
+    <t>17.5000</t>
+  </si>
+  <si>
+    <t>14.7500</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x02_Pin</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>Pico USB TP</t>
+  </si>
+  <si>
+    <t>Spring_Loaded_Pins_2mm</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
+  </si>
+  <si>
+    <t>107.0000</t>
+  </si>
+  <si>
+    <t>1.3500</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>RGB_LED_EXT</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
+  </si>
+  <si>
+    <t>18.9000</t>
+  </si>
+  <si>
+    <t>-4.2250</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Raspberry_pi</t>
+  </si>
+  <si>
+    <t>Raspberry PI Compute Module CM4 Nano A</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
+  </si>
+  <si>
+    <t>29.5900</t>
+  </si>
+  <si>
+    <t>18.6800</t>
   </si>
   <si>
     <t>90.0000</t>
-  </si>
-  <si>
-    <t>3.3500</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>J15</t>
-  </si>
-  <si>
-    <t>MIDI IN/OUT</t>
-  </si>
-  <si>
-    <t>PinHeader_2x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>24.8500</t>
-  </si>
-  <si>
-    <t>80.0750</t>
-  </si>
-  <si>
-    <t>6.7800</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J16 J17</t>
-  </si>
-  <si>
-    <t>MIDI OUT J</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>96.0000</t>
-  </si>
-  <si>
-    <t>100.5000</t>
-  </si>
-  <si>
-    <t>11.2000</t>
-  </si>
-  <si>
-    <t>6.7000</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J1 J2</t>
-  </si>
-  <si>
-    <t>MIDI_OUT</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>103.0000</t>
-  </si>
-  <si>
-    <t>17.5000</t>
-  </si>
-  <si>
-    <t>14.7500</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Pico USB TP</t>
-  </si>
-  <si>
-    <t>Spring_Loaded_Pins_2mm</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
-  </si>
-  <si>
-    <t>107.0000</t>
-  </si>
-  <si>
-    <t>1.3500</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>RGB_LED_EXT</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11021.pdf</t>
-  </si>
-  <si>
-    <t>23.5250</t>
-  </si>
-  <si>
-    <t>1.9750</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Raspberry_pi</t>
-  </si>
-  <si>
-    <t>Raspberry PI Compute Module CM4 Nano A</t>
-  </si>
-  <si>
-    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
-  </si>
-  <si>
-    <t>29.5900</t>
-  </si>
-  <si>
-    <t>18.6800</t>
   </si>
   <si>
     <t>49.9600</t>
@@ -2787,7 +2787,7 @@
         <v>183</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>184</v>
+        <v>62</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>38</v>
@@ -2799,33 +2799,33 @@
         <v>40</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="45" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>143</v>
@@ -2849,10 +2849,10 @@
         <v>96</v>
       </c>
       <c r="O22" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="P22" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="Q22" s="10" t="s">
         <v>62</v>
@@ -2870,30 +2870,30 @@
         <v>149</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>130</v>
@@ -2908,7 +2908,7 @@
         <v>31</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M23" s="7" t="s">
         <v>48</v>
@@ -2917,10 +2917,10 @@
         <v>34</v>
       </c>
       <c r="O23" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="P23" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>203</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>37</v>
@@ -2935,33 +2935,33 @@
         <v>40</v>
       </c>
       <c r="U23" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="V23" s="7" t="s">
         <v>204</v>
-      </c>
-      <c r="V23" s="7" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E24" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="G24" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>130</v>
@@ -2976,7 +2976,7 @@
         <v>31</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M24" s="10" t="s">
         <v>48</v>
@@ -2985,10 +2985,10 @@
         <v>34</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q24" s="10" t="s">
         <v>37</v>
@@ -3003,33 +3003,33 @@
         <v>40</v>
       </c>
       <c r="U24" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="V24" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="V24" s="10" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>126</v>
       </c>
       <c r="E25" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>130</v>
@@ -3044,7 +3044,7 @@
         <v>31</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M25" s="7" t="s">
         <v>48</v>
@@ -3053,7 +3053,7 @@
         <v>96</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P25" s="7" t="s">
         <v>85</v>
@@ -3071,33 +3071,33 @@
         <v>40</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>227</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>230</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>143</v>
@@ -3112,7 +3112,7 @@
         <v>31</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M26" s="10" t="s">
         <v>82</v>
@@ -3121,10 +3121,10 @@
         <v>96</v>
       </c>
       <c r="O26" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="P26" s="10" t="s">
         <v>232</v>
-      </c>
-      <c r="P26" s="10" t="s">
-        <v>233</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>62</v>
@@ -3142,12 +3142,12 @@
         <v>148</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>164</v>
@@ -3159,13 +3159,13 @@
         <v>126</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>130</v>
@@ -3180,7 +3180,7 @@
         <v>31</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>170</v>
@@ -3189,13 +3189,13 @@
         <v>96</v>
       </c>
       <c r="O27" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="P27" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="P27" s="7" t="s">
+      <c r="Q27" s="7" t="s">
         <v>240</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>38</v>
@@ -4419,7 +4419,7 @@
         <v>370</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>184</v>
+        <v>240</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@5c6320140fc33604beedab7a0804e45f52e10822 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -887,7 +887,7 @@
     <t>37.8944</t>
   </si>
   <si>
-    <t>88.0944</t>
+    <t>93.4444</t>
   </si>
   <si>
     <t>2.8500</t>
@@ -908,7 +908,7 @@
     <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
   </si>
   <si>
-    <t>90.2694</t>
+    <t>95.3819</t>
   </si>
   <si>
     <t>26</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@1beb9eb3334a34a7e210046bb4cc3329dde0eee2 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -272,7 +272,7 @@
     <t>pedalboard-hw(4)</t>
   </si>
   <si>
-    <t>47.5944</t>
+    <t>49.4944</t>
   </si>
   <si>
     <t>82.9944</t>
@@ -1067,7 +1067,7 @@
     <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
   </si>
   <si>
-    <t>53.2944</t>
+    <t>55.1944</t>
   </si>
   <si>
     <t>84.0444</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@329373046230eb90cfac6330b5614748efeb6bbd 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="402">
   <si>
     <t>Row</t>
   </si>
@@ -149,7 +149,7 @@
     <t>1.8000</t>
   </si>
   <si>
-    <t>C1 C2 C3 C4 C5 C12</t>
+    <t>C1 C2 C3 C4 C5</t>
   </si>
   <si>
     <t>100nF</t>
@@ -158,342 +158,420 @@
     <t>C_0805_2012Metric</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
+  </si>
+  <si>
+    <t>/MIDI</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(5)</t>
+  </si>
+  <si>
+    <t>30.0944</t>
+  </si>
+  <si>
+    <t>104.8944</t>
+  </si>
+  <si>
+    <t>2.9000</t>
+  </si>
+  <si>
+    <t>1.4500</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C16 C17 C20</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(3)</t>
+  </si>
+  <si>
+    <t>140.6444</t>
+  </si>
+  <si>
+    <t>87.1444</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>C13 C14 C15</t>
+  </si>
+  <si>
+    <t>270uF</t>
+  </si>
+  <si>
+    <t>CP_Elec_10x10</t>
+  </si>
+  <si>
+    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/A768MS277M1GLAE022</t>
+  </si>
+  <si>
+    <t>144.7944</t>
+  </si>
+  <si>
+    <t>93.5269</t>
+  </si>
+  <si>
+    <t>270.0000</t>
+  </si>
+  <si>
+    <t>12.0000</t>
+  </si>
+  <si>
+    <t>2.5000</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ComputeModule4-CM4</t>
+  </si>
+  <si>
+    <t>pedalboard</t>
+  </si>
+  <si>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi-4-Compute-Module</t>
+  </si>
+  <si>
+    <t>Pedalboard Library</t>
+  </si>
+  <si>
+    <t>/Audio</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(1)</t>
+  </si>
+  <si>
+    <t>70.9944</t>
+  </si>
+  <si>
+    <t>67.4944</t>
+  </si>
+  <si>
+    <t>37.7000</t>
+  </si>
+  <si>
+    <t>50.7000</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
-  </si>
-  <si>
-    <t>/MIDI</t>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>LED G</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>LED_SMD</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>31.4944</t>
+  </si>
+  <si>
+    <t>62.9944</t>
+  </si>
+  <si>
+    <t>2.8500</t>
+  </si>
+  <si>
+    <t>1.4000</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>LED Y</t>
+  </si>
+  <si>
+    <t>60.9944</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>SK6812</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4</t>
+  </si>
+  <si>
+    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
+  </si>
+  <si>
+    <t>/LEDs</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(4)</t>
+  </si>
+  <si>
+    <t>49.4944</t>
+  </si>
+  <si>
+    <t>82.9944</t>
+  </si>
+  <si>
+    <t>6.4000</t>
+  </si>
+  <si>
+    <t>4.2000</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>100V 0.15A standard switching diode, DO-35</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>Diode_SMD</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>26.5944</t>
+  </si>
+  <si>
+    <t>98.5944</t>
+  </si>
+  <si>
+    <t>3.9000</t>
+  </si>
+  <si>
+    <t>1.1000</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
+  </si>
+  <si>
+    <t>1N5817</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
+  </si>
+  <si>
+    <t>115.6444</t>
+  </si>
+  <si>
+    <t>81.6944</t>
+  </si>
+  <si>
+    <t>6.5000</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>151.6944</t>
+  </si>
+  <si>
+    <t>102.2444</t>
+  </si>
+  <si>
+    <t>5.4000</t>
+  </si>
+  <si>
+    <t>3.4000</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>161.3944</t>
+  </si>
+  <si>
+    <t>100.5944</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>7.9000</t>
+  </si>
+  <si>
+    <t>7.6000</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x01</t>
+  </si>
+  <si>
+    <t>Connector_Generic</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
+  </si>
+  <si>
+    <t>117.0694</t>
+  </si>
+  <si>
+    <t>71.1444</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>1.7000</t>
+  </si>
+  <si>
+    <t>4.2400</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>J3 J9 J10 J11 J12 J15</t>
+  </si>
+  <si>
+    <t>EXP1</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
   </si>
   <si>
     <t>pedalboard-hw(6)</t>
   </si>
   <si>
-    <t>30.0944</t>
-  </si>
-  <si>
-    <t>104.8944</t>
-  </si>
-  <si>
-    <t>2.9000</t>
-  </si>
-  <si>
-    <t>1.4500</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C16 C17 C20</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(3)</t>
-  </si>
-  <si>
-    <t>140.6444</t>
-  </si>
-  <si>
-    <t>87.1444</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
-    <t>C_Polarized</t>
-  </si>
-  <si>
-    <t>C13 C14 C15</t>
-  </si>
-  <si>
-    <t>270uF</t>
-  </si>
-  <si>
-    <t>CP_Elec_10x10</t>
-  </si>
-  <si>
-    <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/A768MS277M1GLAE022</t>
-  </si>
-  <si>
-    <t>144.7944</t>
-  </si>
-  <si>
-    <t>93.5269</t>
-  </si>
-  <si>
-    <t>270.0000</t>
-  </si>
-  <si>
-    <t>12.0000</t>
-  </si>
-  <si>
-    <t>2.5000</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>RGB LED with integrated controller</t>
-  </si>
-  <si>
-    <t>SK6812</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D1 D2 D3 D4</t>
-  </si>
-  <si>
-    <t>LED_SK6812_PLCC4_5.0x5.0mm_P3.2mm</t>
-  </si>
-  <si>
-    <t>LED_SMD</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/product-files/1138/SK6812+LED+datasheet+.pdf</t>
-  </si>
-  <si>
-    <t>/LEDs</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(4)</t>
-  </si>
-  <si>
-    <t>49.4944</t>
-  </si>
-  <si>
-    <t>82.9944</t>
-  </si>
-  <si>
-    <t>6.4000</t>
-  </si>
-  <si>
-    <t>4.2000</t>
-  </si>
-  <si>
-    <t>100V 0.15A standard switching diode, DO-35</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>SM4007</t>
-  </si>
-  <si>
-    <t>D_SOD-123F</t>
-  </si>
-  <si>
-    <t>Diode_SMD</t>
-  </si>
-  <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(1)</t>
-  </si>
-  <si>
-    <t>26.5944</t>
-  </si>
-  <si>
-    <t>98.5944</t>
-  </si>
-  <si>
-    <t>3.9000</t>
-  </si>
-  <si>
-    <t>1.1000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
-  </si>
-  <si>
-    <t>1N5817</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
-    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
-  </si>
-  <si>
-    <t>115.6444</t>
-  </si>
-  <si>
-    <t>81.6944</t>
-  </si>
-  <si>
-    <t>6.5000</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>Fuse_1812_4532Metric</t>
-  </si>
-  <si>
-    <t>Fuse</t>
-  </si>
-  <si>
-    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
-  </si>
-  <si>
-    <t>151.6944</t>
-  </si>
-  <si>
-    <t>102.2444</t>
-  </si>
-  <si>
-    <t>5.4000</t>
-  </si>
-  <si>
-    <t>3.4000</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>J13</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>Pedalboard Library</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>161.3944</t>
-  </si>
-  <si>
-    <t>100.5944</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>7.9000</t>
-  </si>
-  <si>
-    <t>7.6000</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x01, this symbol is compatible with counter-clockwise, top-bottom and odd-even numbering schemes., script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x01</t>
-  </si>
-  <si>
-    <t>Connector_Generic</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>PinHeader_1x02_P2.54mm_Horizontal</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm</t>
-  </si>
-  <si>
-    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/drawing/68015.pdf</t>
-  </si>
-  <si>
-    <t>117.0694</t>
-  </si>
-  <si>
-    <t>71.1444</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>1.7000</t>
-  </si>
-  <si>
-    <t>4.2400</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>J3 J9 J10 J11 J12 J15</t>
-  </si>
-  <si>
-    <t>EXP1</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
     <t>157.6094</t>
   </si>
   <si>
@@ -506,10 +584,7 @@
     <t>19.2300</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>expansion header for Raspberry Pi 2 &amp; 3</t>
+    <t>15</t>
   </si>
   <si>
     <t>Raspberry_Pi_2_3</t>
@@ -527,9 +602,6 @@
     <t>https://www.hifiberry.com/docs/data-sheets/datasheet-dac-adc-pro/</t>
   </si>
   <si>
-    <t>/Audio</t>
-  </si>
-  <si>
     <t>62.6188</t>
   </si>
   <si>
@@ -539,7 +611,7 @@
     <t>55.0150</t>
   </si>
   <si>
-    <t>13</t>
+    <t>16</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -557,9 +629,6 @@
     <t>Led-Ring</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>160.9944</t>
   </si>
   <si>
@@ -569,7 +638,7 @@
     <t>3.3500</t>
   </si>
   <si>
-    <t>14</t>
+    <t>17</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -602,7 +671,7 @@
     <t>6.7000</t>
   </si>
   <si>
-    <t>15</t>
+    <t>18</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -632,7 +701,7 @@
     <t>14.7500</t>
   </si>
   <si>
-    <t>16</t>
+    <t>19</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated</t>
@@ -656,7 +725,7 @@
     <t>1.3500</t>
   </si>
   <si>
-    <t>17</t>
+    <t>20</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -689,427 +758,379 @@
     <t>1.9500</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Raspberry_pi</t>
-  </si>
-  <si>
-    <t>Raspberry PI Compute Module CM4 Nano A</t>
-  </si>
-  <si>
-    <t>https://www.waveshare.com/wiki/CM4-NANO-A</t>
-  </si>
-  <si>
-    <t>31.5844</t>
-  </si>
-  <si>
-    <t>24.6744</t>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>2.2uH</t>
+  </si>
+  <si>
+    <t>L_1210_3225Metric</t>
+  </si>
+  <si>
+    <t>Inductor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
+  </si>
+  <si>
+    <t>137.2944</t>
+  </si>
+  <si>
+    <t>88.3944</t>
+  </si>
+  <si>
+    <t>4.0500</t>
+  </si>
+  <si>
+    <t>2.6500</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>24.6944</t>
+  </si>
+  <si>
+    <t>102.4944</t>
   </si>
   <si>
     <t>90.0000</t>
   </si>
   <si>
+    <t>2.4500</t>
+  </si>
+  <si>
+    <t>0.9500</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_PDQE15-Q24-S5-D</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
+  </si>
+  <si>
+    <t>117.3644</t>
+  </si>
+  <si>
+    <t>54.9986</t>
+  </si>
+  <si>
+    <t>22.5700</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
+  </si>
+  <si>
+    <t>103.6944</t>
+  </si>
+  <si>
+    <t>4.4150</t>
+  </si>
+  <si>
+    <t>7.4000</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>Resistor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>37.8944</t>
+  </si>
+  <si>
+    <t>93.4444</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>95.3819</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R1 R5</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>22.9944</t>
+  </si>
+  <si>
+    <t>102.3944</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R2 R6</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>31.5444</t>
+  </si>
+  <si>
+    <t>59.0444</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SW4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>11.9944</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>6.8000</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>SW5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>86.9944</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>SW6</t>
+  </si>
+  <si>
+    <t>161.9944</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>63.9944</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>SW3</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>GAIN Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>117.2444</t>
+  </si>
+  <si>
+    <t>99.4944</t>
+  </si>
+  <si>
+    <t>16.5000</t>
+  </si>
+  <si>
+    <t>14.4000</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>VOL Rotary</t>
+  </si>
+  <si>
+    <t>42.2444</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U3 U4</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>55.1944</t>
+  </si>
+  <si>
+    <t>84.0444</t>
+  </si>
+  <si>
+    <t>2.5500</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Pico</t>
+  </si>
+  <si>
+    <t>MCU_RaspberryPi_and_Boards</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>RPi_Pico_SMD_TH</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
+  </si>
+  <si>
+    <t>84.9944</t>
+  </si>
+  <si>
+    <t>81.9944</t>
+  </si>
+  <si>
+    <t>19.4800</t>
+  </si>
+  <si>
     <t>49.9600</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>USB Type A connector</t>
-  </si>
-  <si>
-    <t>USB_A</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>USB A BCB Male Plug</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/GCT%20PDFs/USB1061_Spec.pdf</t>
-  </si>
-  <si>
-    <t>95.6194</t>
-  </si>
-  <si>
-    <t>33.2144</t>
-  </si>
-  <si>
-    <t>9.3200</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>L_1210_3225Metric</t>
-  </si>
-  <si>
-    <t>Inductor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/product-datasheets/srp3212.pdf</t>
-  </si>
-  <si>
-    <t>137.2944</t>
-  </si>
-  <si>
-    <t>88.3944</t>
-  </si>
-  <si>
-    <t>4.0500</t>
-  </si>
-  <si>
-    <t>2.6500</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4 L5</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(5)</t>
-  </si>
-  <si>
-    <t>24.6944</t>
-  </si>
-  <si>
-    <t>102.4944</t>
-  </si>
-  <si>
-    <t>2.4500</t>
-  </si>
-  <si>
-    <t>0.9500</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>PS1</t>
-  </si>
-  <si>
-    <t>CONV_PDQE15-Q24-S5-D</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/pdqe15-d.pdf</t>
-  </si>
-  <si>
-    <t>117.3644</t>
-  </si>
-  <si>
-    <t>54.9986</t>
-  </si>
-  <si>
-    <t>22.5700</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://rocelec.widen.net/view/pdf/rwygqx6rjd/FAIRS27615-1.pdf</t>
-  </si>
-  <si>
-    <t>103.6944</t>
-  </si>
-  <si>
-    <t>4.4150</t>
-  </si>
-  <si>
-    <t>7.4000</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>Resistor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>37.8944</t>
-  </si>
-  <si>
-    <t>93.4444</t>
-  </si>
-  <si>
-    <t>2.8500</t>
-  </si>
-  <si>
-    <t>1.4000</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>95.3819</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>R1 R5</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>22.9944</t>
-  </si>
-  <si>
-    <t>102.3944</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>SW4</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>11.9944</t>
-  </si>
-  <si>
-    <t>16.0000</t>
-  </si>
-  <si>
-    <t>6.8000</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>SW5</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>86.9944</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>SW6</t>
-  </si>
-  <si>
-    <t>161.9944</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>63.9944</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW8</t>
-  </si>
-  <si>
-    <t>GAIN Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>117.2444</t>
-  </si>
-  <si>
-    <t>99.4944</t>
-  </si>
-  <si>
-    <t>16.5000</t>
-  </si>
-  <si>
-    <t>14.4000</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>SW7</t>
-  </si>
-  <si>
-    <t>VOL Rotary</t>
-  </si>
-  <si>
-    <t>42.2444</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOT65P210X110-5N</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>55.1944</t>
-  </si>
-  <si>
-    <t>84.0444</t>
-  </si>
-  <si>
-    <t>3.0480</t>
-  </si>
-  <si>
-    <t>1.6764</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Pico</t>
-  </si>
-  <si>
-    <t>MCU_RaspberryPi_and_Boards</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
-  </si>
-  <si>
-    <t>84.9944</t>
-  </si>
-  <si>
-    <t>81.9944</t>
-  </si>
-  <si>
-    <t>19.4800</t>
-  </si>
-  <si>
-    <t>37</t>
+    <t>39</t>
   </si>
   <si>
     <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
@@ -1181,7 +1202,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>69 (40 SMD/ 27 THT)</t>
+    <t>71 (44 SMD/ 25 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -1699,7 +1720,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1734,7 +1755,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1758,55 +1779,55 @@
     </row>
     <row r="2" spans="1:22">
       <c r="C2" s="2" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="F2" s="3">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="C3" s="2" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="2" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="2" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1814,16 +1835,16 @@
     </row>
     <row r="6" spans="1:22">
       <c r="C6" s="2" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="F6" s="3">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -2166,57 +2187,57 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="30" customHeight="1">
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="I13" s="5" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="O13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="P13" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O13" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="Q13" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>38</v>
@@ -2228,36 +2249,36 @@
         <v>40</v>
       </c>
       <c r="U13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="V13" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="30" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="H14" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>94</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>22</v>
@@ -2268,23 +2289,23 @@
       <c r="K14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="P14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="M14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="O14" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="Q14" s="10" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>38</v>
@@ -2296,36 +2317,36 @@
         <v>40</v>
       </c>
       <c r="U14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="V14" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="30" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="G15" s="7" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>22</v>
@@ -2336,23 +2357,23 @@
       <c r="K15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="7" t="s">
-        <v>107</v>
+      <c r="L15" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>38</v>
@@ -2364,63 +2385,63 @@
         <v>40</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>38</v>
@@ -2432,36 +2453,36 @@
         <v>40</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>22</v>
@@ -2473,63 +2494,63 @@
         <v>31</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="60" customHeight="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>22</v>
@@ -2541,131 +2562,131 @@
         <v>31</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T18" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>22</v>
@@ -2677,471 +2698,471 @@
         <v>31</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>37</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T20" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="V20" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="45" customHeight="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="60" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="11" t="s">
-        <v>179</v>
+      <c r="L21" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="Q21" s="7" t="s">
         <v>61</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T21" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="M22" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R22" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T22" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U22" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="V22" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="30" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="V22" s="10" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
-      <c r="A23" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>199</v>
-      </c>
       <c r="H23" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="T23" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U23" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="45" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="V23" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="30" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="H24" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="10" t="s">
-        <v>210</v>
+      <c r="L24" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>96</v>
+        <v>183</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>85</v>
+        <v>204</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T24" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>218</v>
+        <v>79</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="Q25" s="7" t="s">
         <v>37</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K26" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>230</v>
+        <v>37</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T26" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>149</v>
+        <v>225</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="H27" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>22</v>
@@ -3153,158 +3174,158 @@
         <v>31</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>239</v>
+        <v>111</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="R27" s="7" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="S27" s="7" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T27" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>148</v>
+        <v>234</v>
       </c>
       <c r="V27" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="30" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="28" spans="1:22">
-      <c r="A28" s="8" t="s">
+      <c r="H28" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="I28" s="8" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="Q28" s="10" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="R28" s="10" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="T28" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="V28" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="30" customHeight="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>260</v>
+        <v>81</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>38</v>
@@ -3316,104 +3337,104 @@
         <v>40</v>
       </c>
       <c r="U29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="30" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="V29" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>269</v>
-      </c>
       <c r="H30" s="10" t="s">
-        <v>130</v>
+        <v>252</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>37</v>
+        <v>267</v>
       </c>
       <c r="R30" s="10" t="s">
         <v>38</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T30" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U30" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="V30" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="V30" s="10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="30" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="H31" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>22</v>
@@ -3425,63 +3446,63 @@
         <v>31</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="M31" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O31" s="7" t="s">
-        <v>69</v>
+        <v>275</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="T31" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U31" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="30" customHeight="1">
+      <c r="A32" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="V31" s="7" t="s">
+      <c r="F32" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G32" s="10" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>286</v>
-      </c>
       <c r="H32" s="10" t="s">
-        <v>287</v>
+        <v>79</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>22</v>
@@ -3493,19 +3514,19 @@
         <v>31</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>289</v>
+        <v>69</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>61</v>
@@ -3520,36 +3541,36 @@
         <v>40</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="V32" s="10" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>295</v>
+        <v>127</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>22</v>
@@ -3561,22 +3582,22 @@
         <v>31</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>38</v>
@@ -3588,63 +3609,63 @@
         <v>40</v>
       </c>
       <c r="U33" s="7" t="s">
-        <v>291</v>
+        <v>96</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>292</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>31</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="M34" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="R34" s="10" t="s">
         <v>38</v>
@@ -3656,63 +3677,63 @@
         <v>40</v>
       </c>
       <c r="U34" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="V34" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="V34" s="10" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" ht="30" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="I35" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>38</v>
@@ -3724,60 +3745,60 @@
         <v>40</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>312</v>
+        <v>96</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" ht="30" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="8" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="E36" s="10" t="s">
-        <v>315</v>
-      </c>
       <c r="F36" s="10" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>130</v>
+        <v>291</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L36" s="10" t="s">
-        <v>310</v>
+      <c r="L36" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Q36" s="10" t="s">
         <v>61</v>
@@ -3792,36 +3813,36 @@
         <v>40</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>312</v>
+        <v>96</v>
       </c>
       <c r="V36" s="10" t="s">
-        <v>313</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:22" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>24</v>
+        <v>315</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>22</v>
@@ -3833,19 +3854,19 @@
         <v>31</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="M37" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P37" s="7" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="Q37" s="7" t="s">
         <v>61</v>
@@ -3860,10 +3881,10 @@
         <v>40</v>
       </c>
       <c r="U37" s="7" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:22" ht="30" customHeight="1">
@@ -3871,13 +3892,13 @@
         <v>321</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>322</v>
@@ -3886,10 +3907,10 @@
         <v>323</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>22</v>
@@ -3901,19 +3922,19 @@
         <v>31</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="M38" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="Q38" s="10" t="s">
         <v>61</v>
@@ -3928,10 +3949,10 @@
         <v>40</v>
       </c>
       <c r="U38" s="10" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="V38" s="10" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="30" customHeight="1">
@@ -3939,25 +3960,25 @@
         <v>325</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>326</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>327</v>
+        <v>24</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>22</v>
@@ -3969,19 +3990,19 @@
         <v>31</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="M39" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="Q39" s="7" t="s">
         <v>61</v>
@@ -3996,10 +4017,10 @@
         <v>40</v>
       </c>
       <c r="U39" s="7" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="30" customHeight="1">
@@ -4007,13 +4028,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>329</v>
@@ -4022,10 +4043,10 @@
         <v>330</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>22</v>
@@ -4037,19 +4058,19 @@
         <v>31</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="M40" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P40" s="10" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="Q40" s="10" t="s">
         <v>61</v>
@@ -4064,36 +4085,36 @@
         <v>40</v>
       </c>
       <c r="U40" s="10" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="V40" s="10" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>334</v>
-      </c>
       <c r="G41" s="7" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>22</v>
@@ -4105,19 +4126,19 @@
         <v>31</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="M41" s="7" t="s">
         <v>48</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O41" s="7" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="P41" s="7" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="Q41" s="7" t="s">
         <v>61</v>
@@ -4126,42 +4147,42 @@
         <v>38</v>
       </c>
       <c r="S41" s="7" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T41" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>25</v>
+        <v>313</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>335</v>
+        <v>316</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>22</v>
@@ -4173,19 +4194,19 @@
         <v>31</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="M42" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O42" s="10" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="Q42" s="10" t="s">
         <v>61</v>
@@ -4194,42 +4215,42 @@
         <v>38</v>
       </c>
       <c r="S42" s="10" t="s">
-        <v>134</v>
+        <v>39</v>
       </c>
       <c r="T42" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U42" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="V42" s="10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="30" customHeight="1">
+      <c r="A43" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="V42" s="10" t="s">
+      <c r="D43" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="A43" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>347</v>
-      </c>
       <c r="F43" s="7" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>22</v>
@@ -4241,63 +4262,63 @@
         <v>31</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="M43" s="7" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O43" s="7" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>38</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="30" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>354</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>266</v>
+        <v>348</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>338</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>356</v>
+        <v>25</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>22</v>
@@ -4309,90 +4330,90 @@
         <v>31</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="M44" s="10" t="s">
         <v>48</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="O44" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="Q44" s="10" t="s">
-        <v>230</v>
+        <v>61</v>
       </c>
       <c r="R44" s="10" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="S44" s="10" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="T44" s="10" t="s">
         <v>40</v>
       </c>
       <c r="U44" s="10" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="V44" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="30" customHeight="1">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>364</v>
+        <v>352</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>369</v>
+        <v>355</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="M45" s="7" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="O45" s="7" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>98</v>
+        <v>358</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>38</v>
@@ -4404,10 +4425,146 @@
         <v>40</v>
       </c>
       <c r="U45" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="30" customHeight="1">
+      <c r="A46" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="M46" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="N46" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q46" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="R46" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="S46" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="T46" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="U46" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="V46" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="30" customHeight="1">
+      <c r="A47" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="V45" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>373</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T47" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4433,22 +4590,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="11" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@d17e227001aed1fdd2b0ca74bcede5b0c660dd07 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="528">
   <si>
     <t>Row</t>
   </si>
@@ -169,210 +169,219 @@
     <t>1n</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B102KBANNNC/3886678</t>
+  </si>
+  <si>
+    <t>/Power Supply</t>
+  </si>
+  <si>
+    <t>141.6344</t>
+  </si>
+  <si>
+    <t>83.8844</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>1.2n</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM2165C2A122JA01-01.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/GRM2165C2A122JA01D/2544699</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(1)</t>
+  </si>
+  <si>
+    <t>142.6644</t>
+  </si>
+  <si>
+    <t>81.1744</t>
+  </si>
+  <si>
+    <t>90.0000</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>C1 C11 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C28 C36 C39</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(16)</t>
+  </si>
+  <si>
+    <t>30.0944</t>
+  </si>
+  <si>
+    <t>104.8944</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C15 C17</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
+  </si>
+  <si>
+    <t>84.1944</t>
+  </si>
+  <si>
+    <t>90.4944</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(15)</t>
+  </si>
+  <si>
+    <t>143.2044</t>
+  </si>
+  <si>
+    <t>95.2844</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>100u</t>
+  </si>
+  <si>
+    <t>CP_EIA-7343-31_Kemet-D</t>
+  </si>
+  <si>
+    <t>Capacitor_Tantalum_SMD</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/ABE0000/ABE0000C49.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
+  </si>
+  <si>
+    <t>136.2544</t>
+  </si>
+  <si>
+    <t>75.8644</t>
+  </si>
+  <si>
+    <t>8.3000</t>
+  </si>
+  <si>
+    <t>2.5500</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>/Power Supply</t>
-  </si>
-  <si>
-    <t>141.6344</t>
-  </si>
-  <si>
-    <t>83.8844</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>1.2n</t>
-  </si>
-  <si>
-    <t>http://www.farnell.com/datasheets/2734135.pdf?_ga=2.259347658.1738794919.1588350964-1787849031.1568210898&amp;_gac=1.15394434.1588350964.EAIaIQobChMIgrHHs4yT6QIVxevtCh39TA_nEAAYASAAEgK8PfD_BwE</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(1)</t>
-  </si>
-  <si>
-    <t>142.6644</t>
-  </si>
-  <si>
-    <t>81.1744</t>
-  </si>
-  <si>
-    <t>90.0000</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>C1 C11 C12 C13 C14 C16 C18 C19 C20 C21 C22 C25 C27 C28 C36 C39</t>
-  </si>
-  <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(16)</t>
-  </si>
-  <si>
-    <t>30.0944</t>
-  </si>
-  <si>
-    <t>104.8944</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C15 C17</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
-  </si>
-  <si>
-    <t>84.1944</t>
-  </si>
-  <si>
-    <t>90.4944</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C29 C30 C33 C35 C38</t>
-  </si>
-  <si>
-    <t>10u 35v</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/en-global/products/productdetail.aspx?partno=GRM21BC8YA106ME11%23</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21A226MAYNNNE/10479857</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(15)</t>
-  </si>
-  <si>
-    <t>143.2044</t>
-  </si>
-  <si>
-    <t>95.2844</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>CP_EIA-7343-31_Kemet-D</t>
-  </si>
-  <si>
-    <t>Capacitor_Tantalum_SMD</t>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>pedalboard</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi-4-Compute-Module</t>
+  </si>
+  <si>
+    <t>Pedalboard Library</t>
+  </si>
+  <si>
+    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
+  </si>
+  <si>
+    <t>/Audio</t>
+  </si>
+  <si>
+    <t>70.9944</t>
+  </si>
+  <si>
+    <t>67.4944</t>
+  </si>
+  <si>
+    <t>37.7000</t>
+  </si>
+  <si>
+    <t>50.7000</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>LED R</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>LED_SMD</t>
   </si>
   <si>
     <t>~</t>
   </si>
   <si>
-    <t>136.2544</t>
-  </si>
-  <si>
-    <t>75.8644</t>
-  </si>
-  <si>
-    <t>8.3000</t>
-  </si>
-  <si>
-    <t>2.5500</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>CM4</t>
-  </si>
-  <si>
-    <t>pedalboard</t>
-  </si>
-  <si>
-    <t>CM1</t>
-  </si>
-  <si>
-    <t>Raspberry-Pi-4-Compute-Module</t>
-  </si>
-  <si>
-    <t>Pedalboard Library</t>
-  </si>
-  <si>
-    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
-  </si>
-  <si>
-    <t>/Audio</t>
-  </si>
-  <si>
-    <t>70.9944</t>
-  </si>
-  <si>
-    <t>67.4944</t>
-  </si>
-  <si>
-    <t>37.7000</t>
-  </si>
-  <si>
-    <t>50.7000</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>LED R</t>
-  </si>
-  <si>
-    <t>LED_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>LED_SMD</t>
-  </si>
-  <si>
     <t>31.4944</t>
   </si>
   <si>
@@ -868,6 +877,9 @@
     <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
     <t>146.8944</t>
   </si>
   <si>
@@ -1030,10 +1042,10 @@
     <t>R14 R17</t>
   </si>
   <si>
-    <t>2.2K 1%</t>
-  </si>
-  <si>
-    <t>https://fscdn.rohm.com/en/products/databook/datasheet/passive/resistor/chip_resistor/mcr-e.pdf</t>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
   </si>
   <si>
     <t>137.8244</t>
@@ -1048,7 +1060,10 @@
     <t>R13</t>
   </si>
   <si>
-    <t>12K 1%</t>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
   </si>
   <si>
     <t>135.9044</t>
@@ -1063,7 +1078,10 @@
     <t>R15</t>
   </si>
   <si>
-    <t>20K 1%</t>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
   </si>
   <si>
     <t>140.6644</t>
@@ -1202,6 +1220,9 @@
   </si>
   <si>
     <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
   </si>
   <si>
     <t>141.5144</t>
@@ -2167,7 +2188,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2192,13 +2213,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -2206,41 +2227,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2248,13 +2269,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="F6" s="3">
         <v>106</v>
@@ -2402,7 +2423,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" ht="30" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -2436,10 +2457,10 @@
       <c r="K10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" s="11" t="s">
+      <c r="L10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="9" t="s">
         <v>49</v>
       </c>
       <c r="N10" s="10" t="s">
@@ -2473,7 +2494,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="60" customHeight="1">
+    <row r="11" spans="1:23" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
@@ -2510,23 +2531,23 @@
       <c r="L11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>49</v>
+      <c r="M11" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S11" s="7" t="s">
         <v>40</v>
@@ -2546,7 +2567,7 @@
     </row>
     <row r="12" spans="1:23" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>24</v>
@@ -2558,10 +2579,10 @@
         <v>26</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>29</v>
@@ -2570,10 +2591,10 @@
         <v>30</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>32</v>
@@ -2582,19 +2603,19 @@
         <v>33</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R12" s="10" t="s">
         <v>39</v>
@@ -2617,7 +2638,7 @@
     </row>
     <row r="13" spans="1:23" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>24</v>
@@ -2629,10 +2650,10 @@
         <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>29</v>
@@ -2653,7 +2674,7 @@
         <v>33</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>35</v>
@@ -2662,10 +2683,10 @@
         <v>36</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>39</v>
@@ -2688,7 +2709,7 @@
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>45</v>
@@ -2700,10 +2721,10 @@
         <v>26</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>29</v>
@@ -2712,16 +2733,16 @@
         <v>30</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>81</v>
@@ -2757,7 +2778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
@@ -2791,26 +2812,26 @@
       <c r="K15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M15" s="12" t="s">
-        <v>49</v>
+      <c r="M15" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S15" s="7" t="s">
         <v>40</v>
@@ -2822,36 +2843,36 @@
         <v>42</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="45" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E16" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>23</v>
@@ -2863,22 +2884,22 @@
         <v>32</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>39</v>
@@ -2893,36 +2914,36 @@
         <v>42</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>23</v>
@@ -2934,22 +2955,22 @@
         <v>32</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>39</v>
@@ -2964,36 +2985,36 @@
         <v>42</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>23</v>
@@ -3005,22 +3026,22 @@
         <v>32</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="R18" s="10" t="s">
         <v>39</v>
@@ -3035,63 +3056,63 @@
         <v>42</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>53</v>
@@ -3106,36 +3127,36 @@
         <v>42</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>23</v>
@@ -3147,25 +3168,25 @@
         <v>32</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S20" s="10" t="s">
         <v>40</v>
@@ -3177,36 +3198,36 @@
         <v>42</v>
       </c>
       <c r="V20" s="10" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="W20" s="10" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>31</v>
@@ -3218,10 +3239,10 @@
         <v>32</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="N21" s="7" t="s">
         <v>50</v>
@@ -3230,13 +3251,13 @@
         <v>36</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S21" s="7" t="s">
         <v>40</v>
@@ -3248,36 +3269,36 @@
         <v>42</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="W21" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>23</v>
@@ -3289,22 +3310,22 @@
         <v>32</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P22" s="10" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="R22" s="10" t="s">
         <v>39</v>
@@ -3319,36 +3340,36 @@
         <v>42</v>
       </c>
       <c r="V22" s="10" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -3360,22 +3381,22 @@
         <v>32</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="N23" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="Q23" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>39</v>
@@ -3384,42 +3405,42 @@
         <v>40</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="W23" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>23</v>
@@ -3431,66 +3452,66 @@
         <v>32</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P24" s="10" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>39</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="T24" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>42</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="45" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>23</v>
@@ -3502,66 +3523,66 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>39</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U25" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>31</v>
@@ -3573,10 +3594,10 @@
         <v>32</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="N26" s="10" t="s">
         <v>35</v>
@@ -3585,10 +3606,10 @@
         <v>36</v>
       </c>
       <c r="P26" s="10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>39</v>
@@ -3597,69 +3618,69 @@
         <v>40</v>
       </c>
       <c r="T26" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>42</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="W26" s="10" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="Q27" s="7" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>53</v>
@@ -3668,69 +3689,69 @@
         <v>40</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="45" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="P28" s="10" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="Q28" s="10" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="R28" s="10" t="s">
         <v>53</v>
@@ -3739,42 +3760,42 @@
         <v>40</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>42</v>
       </c>
       <c r="V28" s="10" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="W28" s="10" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>23</v>
@@ -3786,22 +3807,22 @@
         <v>32</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>39</v>
@@ -3810,69 +3831,69 @@
         <v>40</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="N30" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="R30" s="10" t="s">
         <v>53</v>
@@ -3887,36 +3908,36 @@
         <v>42</v>
       </c>
       <c r="V30" s="10" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="W30" s="10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>23</v>
@@ -3928,25 +3949,25 @@
         <v>32</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>49</v>
+        <v>284</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P31" s="7" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S31" s="7" t="s">
         <v>40</v>
@@ -3958,36 +3979,36 @@
         <v>42</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="W31" s="7" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>23</v>
@@ -3999,22 +4020,22 @@
         <v>32</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="N32" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P32" s="10" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="R32" s="10" t="s">
         <v>53</v>
@@ -4029,36 +4050,36 @@
         <v>42</v>
       </c>
       <c r="V32" s="10" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="W32" s="10" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>31</v>
@@ -4070,10 +4091,10 @@
         <v>32</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="N33" s="7" t="s">
         <v>35</v>
@@ -4082,10 +4103,10 @@
         <v>36</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>53</v>
@@ -4100,36 +4121,36 @@
         <v>42</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W33" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>31</v>
@@ -4141,10 +4162,10 @@
         <v>32</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="N34" s="10" t="s">
         <v>35</v>
@@ -4153,10 +4174,10 @@
         <v>36</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="R34" s="10" t="s">
         <v>53</v>
@@ -4171,36 +4192,36 @@
         <v>42</v>
       </c>
       <c r="V34" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>23</v>
@@ -4212,22 +4233,22 @@
         <v>32</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>39</v>
@@ -4242,36 +4263,36 @@
         <v>42</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>31</v>
@@ -4283,10 +4304,10 @@
         <v>32</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="N36" s="10" t="s">
         <v>35</v>
@@ -4295,13 +4316,13 @@
         <v>36</v>
       </c>
       <c r="P36" s="10" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S36" s="10" t="s">
         <v>40</v>
@@ -4313,63 +4334,63 @@
         <v>42</v>
       </c>
       <c r="V36" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="N37" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="P37" s="7" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="Q37" s="7" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="R37" s="7" t="s">
         <v>53</v>
@@ -4384,36 +4405,36 @@
         <v>42</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>31</v>
@@ -4425,10 +4446,10 @@
         <v>32</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>328</v>
+        <v>341</v>
       </c>
       <c r="N38" s="10" t="s">
         <v>50</v>
@@ -4437,13 +4458,13 @@
         <v>36</v>
       </c>
       <c r="P38" s="10" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="Q38" s="10" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="R38" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S38" s="10" t="s">
         <v>40</v>
@@ -4455,36 +4476,36 @@
         <v>42</v>
       </c>
       <c r="V38" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="30" customHeight="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="A39" s="5" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>23</v>
@@ -4496,25 +4517,25 @@
         <v>32</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N39" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O39" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P39" s="7" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="R39" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S39" s="7" t="s">
         <v>40</v>
@@ -4526,36 +4547,36 @@
         <v>42</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W39" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>23</v>
@@ -4567,25 +4588,25 @@
         <v>32</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="M40" s="11" t="s">
-        <v>49</v>
+        <v>314</v>
+      </c>
+      <c r="M40" s="9" t="s">
+        <v>353</v>
       </c>
       <c r="N40" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O40" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P40" s="10" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="Q40" s="10" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="R40" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S40" s="10" t="s">
         <v>40</v>
@@ -4597,36 +4618,36 @@
         <v>42</v>
       </c>
       <c r="V40" s="10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>31</v>
@@ -4638,10 +4659,10 @@
         <v>32</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="N41" s="7" t="s">
         <v>35</v>
@@ -4650,10 +4671,10 @@
         <v>36</v>
       </c>
       <c r="P41" s="7" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="Q41" s="7" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="R41" s="7" t="s">
         <v>53</v>
@@ -4662,69 +4683,69 @@
         <v>40</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="W41" s="7" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="N42" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O42" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="Q42" s="10" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="R42" s="10" t="s">
         <v>53</v>
@@ -4739,36 +4760,36 @@
         <v>42</v>
       </c>
       <c r="V42" s="10" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="W42" s="10" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>31</v>
@@ -4780,22 +4801,22 @@
         <v>32</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="O43" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>39</v>
@@ -4810,36 +4831,36 @@
         <v>42</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W43" s="7" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="45" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>23</v>
@@ -4851,25 +4872,25 @@
         <v>32</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="M44" s="11" t="s">
-        <v>49</v>
+        <v>399</v>
+      </c>
+      <c r="M44" s="9" t="s">
+        <v>400</v>
       </c>
       <c r="N44" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="Q44" s="10" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="R44" s="10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="S44" s="10" t="s">
         <v>40</v>
@@ -4881,36 +4902,36 @@
         <v>42</v>
       </c>
       <c r="V44" s="10" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="W44" s="10" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>23</v>
@@ -4922,22 +4943,22 @@
         <v>32</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>50</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P45" s="7" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="Q45" s="7" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>39</v>
@@ -4952,36 +4973,36 @@
         <v>42</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>23</v>
@@ -4993,25 +5014,25 @@
         <v>32</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="N46" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P46" s="10" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="Q46" s="10" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="R46" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S46" s="10" t="s">
         <v>40</v>
@@ -5023,36 +5044,36 @@
         <v>42</v>
       </c>
       <c r="V46" s="10" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="W46" s="10" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>23</v>
@@ -5064,22 +5085,22 @@
         <v>32</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O47" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P47" s="7" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>53</v>
@@ -5094,36 +5115,36 @@
         <v>42</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>23</v>
@@ -5135,25 +5156,25 @@
         <v>32</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="N48" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O48" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P48" s="10" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="Q48" s="10" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="R48" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S48" s="10" t="s">
         <v>40</v>
@@ -5165,36 +5186,36 @@
         <v>42</v>
       </c>
       <c r="V48" s="10" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="W48" s="10" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
     </row>
     <row r="49" spans="1:23" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>23</v>
@@ -5206,22 +5227,22 @@
         <v>32</v>
       </c>
       <c r="L49" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O49" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P49" s="7" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="Q49" s="7" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="R49" s="7" t="s">
         <v>53</v>
@@ -5236,10 +5257,10 @@
         <v>42</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="W49" s="7" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -5290,7 +5311,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5315,13 +5336,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -5329,41 +5350,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5371,13 +5392,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="F6" s="3">
         <v>106</v>
@@ -5459,40 +5480,40 @@
         <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>35</v>
@@ -5501,10 +5522,10 @@
         <v>36</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>39</v>
@@ -5516,13 +5537,13 @@
         <v>41</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -5530,40 +5551,40 @@
         <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>35</v>
@@ -5572,28 +5593,28 @@
         <v>36</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="Q10" s="10" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S10" s="10" t="s">
         <v>40</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="45" customHeight="1">
@@ -5601,40 +5622,40 @@
         <v>54</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="N11" s="7" t="s">
         <v>35</v>
@@ -5643,152 +5664,152 @@
         <v>36</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>39</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S12" s="10" t="s">
         <v>40</v>
       </c>
       <c r="T12" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>53</v>
@@ -5800,54 +5821,54 @@
         <v>41</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="N14" s="10" t="s">
         <v>35</v>
@@ -5856,13 +5877,13 @@
         <v>36</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S14" s="10" t="s">
         <v>40</v>
@@ -5871,13 +5892,13 @@
         <v>41</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="W14" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -5903,22 +5924,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="12" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@0edb0cb26a37e28591dca158c81390d0ae3dad52 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -1216,106 +1216,106 @@
     <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
   </si>
   <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+  </si>
+  <si>
+    <t>141.5144</t>
+  </si>
+  <si>
+    <t>88.5944</t>
+  </si>
+  <si>
+    <t>6.9000</t>
+  </si>
+  <si>
+    <t>4.9000</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>Regulator_Linear</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>115.6444</t>
+  </si>
+  <si>
+    <t>74.1444</t>
+  </si>
+  <si>
+    <t>6.1000</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>89.3944</t>
+  </si>
+  <si>
+    <t>85.3944</t>
+  </si>
+  <si>
+    <t>7.7500</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>Isolator</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
     <t>Package_SO</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
-  </si>
-  <si>
-    <t>141.5144</t>
-  </si>
-  <si>
-    <t>88.5944</t>
-  </si>
-  <si>
-    <t>6.9000</t>
-  </si>
-  <si>
-    <t>4.9000</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>Regulator_Linear</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>115.6444</t>
-  </si>
-  <si>
-    <t>74.1444</t>
-  </si>
-  <si>
-    <t>6.1000</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>89.3944</t>
-  </si>
-  <si>
-    <t>85.3944</t>
-  </si>
-  <si>
-    <t>7.7500</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>Isolator</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
   </si>
   <si>
     <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
@@ -4863,7 +4863,7 @@
         <v>397</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>398</v>
+        <v>104</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>23</v>
@@ -4875,10 +4875,10 @@
         <v>32</v>
       </c>
       <c r="L44" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="M44" s="9" t="s">
         <v>399</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>400</v>
       </c>
       <c r="N44" s="10" t="s">
         <v>50</v>
@@ -4887,10 +4887,10 @@
         <v>59</v>
       </c>
       <c r="P44" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q44" s="10" t="s">
         <v>401</v>
-      </c>
-      <c r="Q44" s="10" t="s">
-        <v>402</v>
       </c>
       <c r="R44" s="10" t="s">
         <v>153</v>
@@ -4905,33 +4905,33 @@
         <v>42</v>
       </c>
       <c r="V44" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="W44" s="10" t="s">
         <v>403</v>
-      </c>
-      <c r="W44" s="10" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>409</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>410</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>386</v>
@@ -4946,10 +4946,10 @@
         <v>32</v>
       </c>
       <c r="L45" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>412</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>50</v>
@@ -4958,10 +4958,10 @@
         <v>59</v>
       </c>
       <c r="P45" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q45" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="Q45" s="7" t="s">
-        <v>414</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>39</v>
@@ -4979,30 +4979,30 @@
         <v>96</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>417</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>418</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>419</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>420</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>104</v>
@@ -5017,10 +5017,10 @@
         <v>32</v>
       </c>
       <c r="L46" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>421</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>422</v>
       </c>
       <c r="N46" s="10" t="s">
         <v>35</v>
@@ -5029,10 +5029,10 @@
         <v>59</v>
       </c>
       <c r="P46" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q46" s="10" t="s">
         <v>423</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>424</v>
       </c>
       <c r="R46" s="10" t="s">
         <v>62</v>
@@ -5047,36 +5047,36 @@
         <v>42</v>
       </c>
       <c r="V46" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="W46" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>428</v>
-      </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>431</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>398</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@71cc22228b63dacac1e99c41e951aad9e4d50dc7 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -229,10 +229,13 @@
     <t>pedalboard-hw(14)</t>
   </si>
   <si>
-    <t>30.0944</t>
-  </si>
-  <si>
-    <t>104.8944</t>
+    <t>59.7944</t>
+  </si>
+  <si>
+    <t>98.7944</t>
+  </si>
+  <si>
+    <t>270.0000</t>
   </si>
   <si>
     <t>5</t>
@@ -472,13 +475,10 @@
     <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
   </si>
   <si>
-    <t>26.5944</t>
-  </si>
-  <si>
-    <t>98.5944</t>
-  </si>
-  <si>
-    <t>270.0000</t>
+    <t>65.7444</t>
+  </si>
+  <si>
+    <t>87.4544</t>
   </si>
   <si>
     <t>3.9000</t>
@@ -802,10 +802,10 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
   </si>
   <si>
-    <t>63.5344</t>
-  </si>
-  <si>
-    <t>74.7044</t>
+    <t>53.7344</t>
+  </si>
+  <si>
+    <t>75.9644</t>
   </si>
   <si>
     <t>8.0000</t>
@@ -844,10 +844,10 @@
     <t>pedalboard-hw(4)</t>
   </si>
   <si>
-    <t>34.6944</t>
-  </si>
-  <si>
-    <t>95.3319</t>
+    <t>62.3844</t>
+  </si>
+  <si>
+    <t>79.3544</t>
   </si>
   <si>
     <t>2.4500</t>
@@ -952,10 +952,10 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
-    <t>37.8944</t>
-  </si>
-  <si>
-    <t>93.4444</t>
+    <t>60.7244</t>
+  </si>
+  <si>
+    <t>76.1544</t>
   </si>
   <si>
     <t>26</t>
@@ -991,7 +991,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
-    <t>95.3819</t>
+    <t>62.6244</t>
   </si>
   <si>
     <t>28</t>
@@ -1006,10 +1006,10 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
   </si>
   <si>
-    <t>22.9944</t>
-  </si>
-  <si>
-    <t>102.3944</t>
+    <t>67.2844</t>
+  </si>
+  <si>
+    <t>91.0144</t>
   </si>
   <si>
     <t>29</t>
@@ -1327,7 +1327,7 @@
     <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
-    <t>33.3944</t>
+    <t>80.6544</t>
   </si>
   <si>
     <t>10.8000</t>
@@ -1528,10 +1528,10 @@
     <t>J23 J24</t>
   </si>
   <si>
-    <t>31.5944</t>
-  </si>
-  <si>
-    <t>102.5194</t>
+    <t>52.6344</t>
+  </si>
+  <si>
+    <t>107.3844</t>
   </si>
   <si>
     <t>Generic screw terminal, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -2624,7 +2624,7 @@
         <v>70</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="S12" s="10" t="s">
         <v>40</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="13" spans="1:23" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>24</v>
@@ -2656,10 +2656,10 @@
         <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>29</v>
@@ -2680,7 +2680,7 @@
         <v>33</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>35</v>
@@ -2689,10 +2689,10 @@
         <v>36</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>39</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>45</v>
@@ -2727,10 +2727,10 @@
         <v>26</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>29</v>
@@ -2739,10 +2739,10 @@
         <v>30</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>32</v>
@@ -2751,19 +2751,19 @@
         <v>33</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N14" s="10" t="s">
         <v>50</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P14" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>53</v>
@@ -2786,28 +2786,28 @@
     </row>
     <row r="15" spans="1:23" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>23</v>
@@ -2819,10 +2819,10 @@
         <v>32</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>50</v>
@@ -2831,10 +2831,10 @@
         <v>59</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q15" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>62</v>
@@ -2849,36 +2849,36 @@
         <v>42</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="45" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>23</v>
@@ -2890,22 +2890,22 @@
         <v>32</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>59</v>
       </c>
       <c r="P16" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>39</v>
@@ -2920,36 +2920,36 @@
         <v>42</v>
       </c>
       <c r="V16" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>23</v>
@@ -2961,22 +2961,22 @@
         <v>32</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O17" s="5" t="s">
         <v>59</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q17" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>39</v>
@@ -2991,36 +2991,36 @@
         <v>42</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>23</v>
@@ -3032,22 +3032,22 @@
         <v>32</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>59</v>
       </c>
       <c r="P18" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R18" s="10" t="s">
         <v>39</v>
@@ -3062,36 +3062,36 @@
         <v>42</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W18" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="G19" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>31</v>
@@ -3103,22 +3103,22 @@
         <v>32</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>36</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q19" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>53</v>
@@ -3133,36 +3133,36 @@
         <v>42</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>23</v>
@@ -3174,10 +3174,10 @@
         <v>32</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>35</v>
@@ -3186,13 +3186,13 @@
         <v>59</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Q20" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="S20" s="10" t="s">
         <v>40</v>
@@ -3233,7 +3233,7 @@
         <v>160</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>31</v>
@@ -3263,7 +3263,7 @@
         <v>164</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="S21" s="7" t="s">
         <v>40</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="23" spans="1:23" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>179</v>
@@ -3375,7 +3375,7 @@
         <v>184</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>23</v>
@@ -3434,7 +3434,7 @@
         <v>194</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>195</v>
@@ -3446,7 +3446,7 @@
         <v>197</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>23</v>
@@ -3458,13 +3458,13 @@
         <v>32</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O24" s="8" t="s">
         <v>59</v>
@@ -3535,7 +3535,7 @@
         <v>211</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O25" s="5" t="s">
         <v>59</v>
@@ -3588,7 +3588,7 @@
         <v>222</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>31</v>
@@ -3659,13 +3659,13 @@
         <v>233</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>32</v>
@@ -3730,25 +3730,25 @@
         <v>247</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O28" s="8" t="s">
         <v>248</v>
@@ -3789,7 +3789,7 @@
         <v>254</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>255</v>
@@ -3801,7 +3801,7 @@
         <v>257</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>23</v>
@@ -3831,7 +3831,7 @@
         <v>261</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="S29" s="7" t="s">
         <v>40</v>
@@ -3902,7 +3902,7 @@
         <v>275</v>
       </c>
       <c r="R30" s="10" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="S30" s="10" t="s">
         <v>40</v>
@@ -3973,7 +3973,7 @@
         <v>288</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="S31" s="7" t="s">
         <v>40</v>
@@ -4002,7 +4002,7 @@
         <v>292</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>293</v>
@@ -4014,7 +4014,7 @@
         <v>294</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>23</v>
@@ -4115,7 +4115,7 @@
         <v>311</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="S33" s="7" t="s">
         <v>40</v>
@@ -4127,10 +4127,10 @@
         <v>42</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W33" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="30" customHeight="1">
@@ -4198,10 +4198,10 @@
         <v>42</v>
       </c>
       <c r="V34" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W34" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="30" customHeight="1">
@@ -4251,13 +4251,13 @@
         <v>59</v>
       </c>
       <c r="P35" s="7" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>40</v>
@@ -4269,10 +4269,10 @@
         <v>42</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="30" customHeight="1">
@@ -4328,7 +4328,7 @@
         <v>329</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="S36" s="10" t="s">
         <v>40</v>
@@ -4340,10 +4340,10 @@
         <v>42</v>
       </c>
       <c r="V36" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W36" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="30" customHeight="1">
@@ -4372,10 +4372,10 @@
         <v>307</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>32</v>
@@ -4411,10 +4411,10 @@
         <v>42</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="30" customHeight="1">
@@ -4482,10 +4482,10 @@
         <v>42</v>
       </c>
       <c r="V38" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W38" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -4526,7 +4526,7 @@
         <v>348</v>
       </c>
       <c r="M39" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N39" s="7" t="s">
         <v>50</v>
@@ -4553,10 +4553,10 @@
         <v>42</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W39" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30" customHeight="1">
@@ -4612,7 +4612,7 @@
         <v>356</v>
       </c>
       <c r="R40" s="10" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="S40" s="10" t="s">
         <v>40</v>
@@ -4624,10 +4624,10 @@
         <v>42</v>
       </c>
       <c r="V40" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W40" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="30" customHeight="1">
@@ -4653,7 +4653,7 @@
         <v>362</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>31</v>
@@ -4724,13 +4724,13 @@
         <v>375</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>32</v>
@@ -4783,7 +4783,7 @@
         <v>384</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>385</v>
@@ -4813,7 +4813,7 @@
         <v>389</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O43" s="5" t="s">
         <v>36</v>
@@ -4837,7 +4837,7 @@
         <v>42</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W43" s="7" t="s">
         <v>392</v>
@@ -4848,7 +4848,7 @@
         <v>393</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>394</v>
@@ -4866,7 +4866,7 @@
         <v>398</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>23</v>
@@ -4896,7 +4896,7 @@
         <v>402</v>
       </c>
       <c r="R44" s="10" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="S44" s="10" t="s">
         <v>40</v>
@@ -4979,7 +4979,7 @@
         <v>42</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W45" s="7" t="s">
         <v>415</v>
@@ -4996,7 +4996,7 @@
         <v>418</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>419</v>
@@ -5008,7 +5008,7 @@
         <v>420</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>23</v>
@@ -5103,13 +5103,13 @@
         <v>59</v>
       </c>
       <c r="P47" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q47" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="Q47" s="7" t="s">
-        <v>151</v>
-      </c>
       <c r="R47" s="7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>40</v>
@@ -5138,7 +5138,7 @@
         <v>440</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E48" s="10" t="s">
         <v>441</v>
@@ -5150,7 +5150,7 @@
         <v>443</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>23</v>
@@ -5221,7 +5221,7 @@
         <v>455</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>23</v>
@@ -5504,7 +5504,7 @@
         <v>484</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>31</v>
@@ -5587,10 +5587,10 @@
         <v>486</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>35</v>
@@ -5676,7 +5676,7 @@
         <v>503</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="S11" s="7" t="s">
         <v>200</v>
@@ -5729,7 +5729,7 @@
         <v>486</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>509</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>302</v>
@@ -5800,10 +5800,10 @@
         <v>486</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N13" s="7" t="s">
         <v>35</v>
@@ -5830,15 +5830,15 @@
         <v>491</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>370</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@9f26bfbdac674d52c2dd905373fbb87f02c0f916 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -610,904 +610,904 @@
     <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
+    <t>127.8644</t>
+  </si>
+  <si>
+    <t>77.1844</t>
+  </si>
+  <si>
+    <t>12.4000</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>71.9889</t>
+  </si>
+  <si>
+    <t>106.4944</t>
+  </si>
+  <si>
+    <t>11.2000</t>
+  </si>
+  <si>
+    <t>6.7000</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J8 J18 J19 J20 J22</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(6)</t>
+  </si>
+  <si>
+    <t>157.6094</t>
+  </si>
+  <si>
+    <t>97.1944</t>
+  </si>
+  <si>
+    <t>15.7000</t>
+  </si>
+  <si>
+    <t>19.2300</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x02_Odd_Even</t>
+  </si>
+  <si>
+    <t>Connector_Generic</t>
+  </si>
+  <si>
+    <t>J9 J10 J13 J15 J17 J21 J23 J24</t>
+  </si>
+  <si>
+    <t>LED-Ring</t>
+  </si>
+  <si>
+    <t>Led-Ring</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(8)</t>
+  </si>
+  <si>
+    <t>10.9944</t>
+  </si>
+  <si>
+    <t>74.9944</t>
+  </si>
+  <si>
+    <t>3.3500</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>Pedalboard Soundcard</t>
+  </si>
+  <si>
+    <t>Pedalboard_Soundcard</t>
+  </si>
+  <si>
+    <t>102.2444</t>
+  </si>
+  <si>
+    <t>62.6188</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>41.4500</t>
+  </si>
+  <si>
+    <t>55.0150</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Inductor with ferrite core</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>Inductor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(4)</t>
+  </si>
+  <si>
+    <t>64.2444</t>
+  </si>
+  <si>
+    <t>89.3344</t>
+  </si>
+  <si>
+    <t>2.4500</t>
+  </si>
+  <si>
+    <t>0.9500</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Inductor symbol for simulation only</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>pspice</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
+    <t>146.8944</t>
+  </si>
+  <si>
+    <t>80.8544</t>
+  </si>
+  <si>
+    <t>5.1000</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>P-Channel MOSFET</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>141.8544</t>
+  </si>
+  <si>
+    <t>102.8344</t>
+  </si>
+  <si>
+    <t>4.4150</t>
+  </si>
+  <si>
+    <t>7.4000</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Resistor, small symbol</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R5 R13</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>Resistor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>60.7244</t>
+  </si>
+  <si>
+    <t>76.1544</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>R6 R10</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>80.1344</t>
+  </si>
+  <si>
+    <t>84.6344</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>62.6244</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R3 R7</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>67.2844</t>
+  </si>
+  <si>
+    <t>91.0144</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R1 R2 R8 R11 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(5)</t>
+  </si>
+  <si>
+    <t>153.0944</t>
+  </si>
+  <si>
+    <t>100.1644</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R15 R17</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
+  </si>
+  <si>
+    <t>137.8244</t>
+  </si>
+  <si>
+    <t>87.2244</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R18 R19</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
+  </si>
+  <si>
+    <t>130.7344</t>
+  </si>
+  <si>
+    <t>86.1844</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
+  </si>
+  <si>
+    <t>135.9044</t>
+  </si>
+  <si>
+    <t>83.8644</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
+  </si>
+  <si>
+    <t>140.6644</t>
+  </si>
+  <si>
+    <t>81.1944</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>42.2444</t>
+  </si>
+  <si>
+    <t>99.4944</t>
+  </si>
+  <si>
+    <t>16.5000</t>
+  </si>
+  <si>
+    <t>14.4000</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>11.9944</t>
+  </si>
+  <si>
+    <t>63.9944</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>6.8000</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Single OR Gage</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U1 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>70.4544</t>
+  </si>
+  <si>
+    <t>78.6444</t>
+  </si>
+  <si>
+    <t>1.7000</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>CM4IO</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+  </si>
+  <si>
+    <t>141.5144</t>
+  </si>
+  <si>
+    <t>88.5944</t>
+  </si>
+  <si>
+    <t>6.9000</t>
+  </si>
+  <si>
+    <t>4.9000</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>Regulator_Linear</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>115.1644</t>
+  </si>
+  <si>
+    <t>74.1444</t>
+  </si>
+  <si>
+    <t>6.1000</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>A microcontroller by Raspberry Pi</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>89.3944</t>
+  </si>
+  <si>
+    <t>85.3944</t>
+  </si>
+  <si>
+    <t>7.7500</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>Isolator</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Package_SO</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>80.6544</t>
+  </si>
+  <si>
+    <t>10.8000</t>
+  </si>
+  <si>
+    <t>3.3400</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>81.4944</t>
+  </si>
+  <si>
+    <t>78.5444</t>
+  </si>
+  <si>
+    <t>8.8000</t>
+  </si>
+  <si>
+    <t>4.4100</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>99.9944</t>
+  </si>
+  <si>
+    <t>74.8944</t>
+  </si>
+  <si>
+    <t>14.6000</t>
+  </si>
+  <si>
+    <t>2.1000</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>3.2.0-RC1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-12-05</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>117 (88 SMD/ 27 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>105 (85 SMD/ 20 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>71.9944</t>
+  </si>
+  <si>
+    <t>108.9944</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>17.5000</t>
+  </si>
+  <si>
+    <t>14.7500</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x03, script generated</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J12 J16</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm</t>
+  </si>
+  <si>
+    <t>111.3094</t>
+  </si>
+  <si>
+    <t>86.5444</t>
+  </si>
+  <si>
+    <t>6.7800</t>
+  </si>
+  <si>
+    <t>J25 J26 J28</t>
+  </si>
+  <si>
+    <t>JST PH 3</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
+  </si>
+  <si>
     <t>Connector_JST</t>
-  </si>
-  <si>
-    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
-  </si>
-  <si>
-    <t>127.8644</t>
-  </si>
-  <si>
-    <t>77.1844</t>
-  </si>
-  <si>
-    <t>12.4000</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>71.9889</t>
-  </si>
-  <si>
-    <t>106.4944</t>
-  </si>
-  <si>
-    <t>11.2000</t>
-  </si>
-  <si>
-    <t>6.7000</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J8 J18 J19 J20 J22</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(6)</t>
-  </si>
-  <si>
-    <t>157.6094</t>
-  </si>
-  <si>
-    <t>97.1944</t>
-  </si>
-  <si>
-    <t>15.7000</t>
-  </si>
-  <si>
-    <t>19.2300</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Generic</t>
-  </si>
-  <si>
-    <t>J9 J10 J13 J15 J17 J21 J23 J24</t>
-  </si>
-  <si>
-    <t>LED-Ring</t>
-  </si>
-  <si>
-    <t>Led-Ring</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(8)</t>
-  </si>
-  <si>
-    <t>10.9944</t>
-  </si>
-  <si>
-    <t>74.9944</t>
-  </si>
-  <si>
-    <t>3.3500</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Sound Card (Based on HifiBerry DAC/ADC pro)</t>
-  </si>
-  <si>
-    <t>Raspberry_Sound_Card</t>
-  </si>
-  <si>
-    <t>J27</t>
-  </si>
-  <si>
-    <t>Pedalboard Soundcard</t>
-  </si>
-  <si>
-    <t>Pedalboard_Soundcard</t>
-  </si>
-  <si>
-    <t>102.2444</t>
-  </si>
-  <si>
-    <t>62.6188</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>41.4500</t>
-  </si>
-  <si>
-    <t>55.0150</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Inductor with ferrite core</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>Inductor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(4)</t>
-  </si>
-  <si>
-    <t>64.2444</t>
-  </si>
-  <si>
-    <t>89.3344</t>
-  </si>
-  <si>
-    <t>2.4500</t>
-  </si>
-  <si>
-    <t>0.9500</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Inductor symbol for simulation only</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>pspice</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
-  </si>
-  <si>
-    <t>146.8944</t>
-  </si>
-  <si>
-    <t>80.8544</t>
-  </si>
-  <si>
-    <t>5.1000</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>P-Channel MOSFET</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>141.8544</t>
-  </si>
-  <si>
-    <t>102.8344</t>
-  </si>
-  <si>
-    <t>4.4150</t>
-  </si>
-  <si>
-    <t>7.4000</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R5 R13</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>Resistor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>60.7244</t>
-  </si>
-  <si>
-    <t>76.1544</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>R6 R10</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>80.1344</t>
-  </si>
-  <si>
-    <t>84.6344</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>62.6244</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>R3 R7</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>67.2844</t>
-  </si>
-  <si>
-    <t>91.0144</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>R1 R2 R8 R11 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(5)</t>
-  </si>
-  <si>
-    <t>153.0944</t>
-  </si>
-  <si>
-    <t>100.1644</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R15 R17</t>
-  </si>
-  <si>
-    <t>2K2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
-  </si>
-  <si>
-    <t>137.8244</t>
-  </si>
-  <si>
-    <t>87.2244</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R18 R19</t>
-  </si>
-  <si>
-    <t>3K9</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
-  </si>
-  <si>
-    <t>130.7344</t>
-  </si>
-  <si>
-    <t>86.1844</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>12K</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
-  </si>
-  <si>
-    <t>135.9044</t>
-  </si>
-  <si>
-    <t>83.8644</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
-  </si>
-  <si>
-    <t>140.6644</t>
-  </si>
-  <si>
-    <t>81.1944</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>42.2444</t>
-  </si>
-  <si>
-    <t>99.4944</t>
-  </si>
-  <si>
-    <t>16.5000</t>
-  </si>
-  <si>
-    <t>14.4000</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
-  </si>
-  <si>
-    <t>Tactile Button</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>11.9944</t>
-  </si>
-  <si>
-    <t>63.9944</t>
-  </si>
-  <si>
-    <t>16.0000</t>
-  </si>
-  <si>
-    <t>6.8000</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Single OR Gage</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U1 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>70.4544</t>
-  </si>
-  <si>
-    <t>78.6444</t>
-  </si>
-  <si>
-    <t>1.7000</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>CM4IO</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
-  </si>
-  <si>
-    <t>141.5144</t>
-  </si>
-  <si>
-    <t>88.5944</t>
-  </si>
-  <si>
-    <t>6.9000</t>
-  </si>
-  <si>
-    <t>4.9000</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>Regulator_Linear</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>115.1644</t>
-  </si>
-  <si>
-    <t>74.1444</t>
-  </si>
-  <si>
-    <t>6.1000</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>A microcontroller by Raspberry Pi</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>89.3944</t>
-  </si>
-  <si>
-    <t>85.3944</t>
-  </si>
-  <si>
-    <t>7.7500</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>Isolator</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>Package_SO</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>80.6544</t>
-  </si>
-  <si>
-    <t>10.8000</t>
-  </si>
-  <si>
-    <t>3.3400</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Flash Memory</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>81.4944</t>
-  </si>
-  <si>
-    <t>78.5444</t>
-  </si>
-  <si>
-    <t>8.8000</t>
-  </si>
-  <si>
-    <t>4.4100</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>99.9944</t>
-  </si>
-  <si>
-    <t>74.8944</t>
-  </si>
-  <si>
-    <t>14.6000</t>
-  </si>
-  <si>
-    <t>2.1000</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>3.2.0-RC1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-12-05</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>117 (88 SMD/ 27 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>105 (85 SMD/ 20 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>71.9944</t>
-  </si>
-  <si>
-    <t>108.9944</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>17.5000</t>
-  </si>
-  <si>
-    <t>14.7500</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x03, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J12 J16</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm</t>
-  </si>
-  <si>
-    <t>111.3094</t>
-  </si>
-  <si>
-    <t>86.5444</t>
-  </si>
-  <si>
-    <t>6.7800</t>
-  </si>
-  <si>
-    <t>J25 J26 J28</t>
-  </si>
-  <si>
-    <t>JST PH 3</t>
-  </si>
-  <si>
-    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
@@ -2221,7 +2221,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>454</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -2260,41 +2260,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>456</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>458</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>466</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>460</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2302,13 +2302,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>462</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -3473,7 +3473,7 @@
         <v>195</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>196</v>
+        <v>102</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>23</v>
@@ -3485,10 +3485,10 @@
         <v>32</v>
       </c>
       <c r="L24" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>198</v>
       </c>
       <c r="N24" s="10" t="s">
         <v>35</v>
@@ -3497,10 +3497,10 @@
         <v>57</v>
       </c>
       <c r="P24" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q24" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="Q24" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="R24" s="10" t="s">
         <v>51</v>
@@ -3515,7 +3515,7 @@
         <v>42</v>
       </c>
       <c r="V24" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="W24" s="10" t="s">
         <v>163</v>
@@ -3523,25 +3523,25 @@
     </row>
     <row r="25" spans="1:23" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>102</v>
@@ -3556,10 +3556,10 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>35</v>
@@ -3568,10 +3568,10 @@
         <v>36</v>
       </c>
       <c r="P25" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>212</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>39</v>
@@ -3586,33 +3586,33 @@
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="W25" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="30" customHeight="1">
       <c r="A26" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>102</v>
@@ -3627,22 +3627,22 @@
         <v>32</v>
       </c>
       <c r="L26" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="M26" s="9" t="s">
         <v>221</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>222</v>
       </c>
       <c r="N26" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O26" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="P26" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="P26" s="10" t="s">
+      <c r="Q26" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="R26" s="10" t="s">
         <v>136</v>
@@ -3657,33 +3657,33 @@
         <v>42</v>
       </c>
       <c r="V26" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="W26" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="W26" s="10" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="45" customHeight="1">
       <c r="A27" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>102</v>
@@ -3707,13 +3707,13 @@
         <v>133</v>
       </c>
       <c r="O27" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="P27" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="P27" s="7" t="s">
+      <c r="Q27" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>136</v>
@@ -3728,33 +3728,33 @@
         <v>42</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>241</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E28" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="G28" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>244</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>102</v>
@@ -3781,16 +3781,16 @@
         <v>57</v>
       </c>
       <c r="P28" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q28" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="Q28" s="10" t="s">
-        <v>246</v>
       </c>
       <c r="R28" s="10" t="s">
         <v>39</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T28" s="10" t="s">
         <v>187</v>
@@ -3799,36 +3799,36 @@
         <v>42</v>
       </c>
       <c r="V28" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="W28" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="W28" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>255</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>60</v>
@@ -3840,22 +3840,22 @@
         <v>32</v>
       </c>
       <c r="L29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="M29" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O29" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="P29" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="P29" s="7" t="s">
+      <c r="Q29" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>39</v>
@@ -3870,36 +3870,36 @@
         <v>42</v>
       </c>
       <c r="V29" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="W29" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="W29" s="7" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="G30" s="10" t="s">
-        <v>270</v>
-      </c>
       <c r="H30" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>23</v>
@@ -3911,10 +3911,10 @@
         <v>32</v>
       </c>
       <c r="L30" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="M30" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>272</v>
       </c>
       <c r="N30" s="10" t="s">
         <v>48</v>
@@ -3923,10 +3923,10 @@
         <v>57</v>
       </c>
       <c r="P30" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q30" s="10" t="s">
         <v>273</v>
-      </c>
-      <c r="Q30" s="10" t="s">
-        <v>274</v>
       </c>
       <c r="R30" s="10" t="s">
         <v>68</v>
@@ -3944,30 +3944,30 @@
         <v>163</v>
       </c>
       <c r="W30" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E31" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>280</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>102</v>
@@ -3982,10 +3982,10 @@
         <v>32</v>
       </c>
       <c r="L31" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>48</v>
@@ -3994,10 +3994,10 @@
         <v>57</v>
       </c>
       <c r="P31" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q31" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>136</v>
@@ -4012,36 +4012,36 @@
         <v>42</v>
       </c>
       <c r="V31" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="W31" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="W31" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="G32" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="H32" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I32" s="8" t="s">
         <v>31</v>
@@ -4053,10 +4053,10 @@
         <v>32</v>
       </c>
       <c r="L32" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="M32" s="9" t="s">
         <v>294</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>295</v>
       </c>
       <c r="N32" s="10" t="s">
         <v>35</v>
@@ -4065,10 +4065,10 @@
         <v>36</v>
       </c>
       <c r="P32" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q32" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="Q32" s="10" t="s">
-        <v>297</v>
       </c>
       <c r="R32" s="10" t="s">
         <v>68</v>
@@ -4091,28 +4091,28 @@
     </row>
     <row r="33" spans="1:23" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>300</v>
-      </c>
       <c r="G33" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>31</v>
@@ -4124,10 +4124,10 @@
         <v>32</v>
       </c>
       <c r="L33" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="M33" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="M33" s="6" t="s">
-        <v>302</v>
       </c>
       <c r="N33" s="7" t="s">
         <v>35</v>
@@ -4136,10 +4136,10 @@
         <v>36</v>
       </c>
       <c r="P33" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q33" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="Q33" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>136</v>
@@ -4162,28 +4162,28 @@
     </row>
     <row r="34" spans="1:23" ht="30" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>307</v>
-      </c>
       <c r="G34" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H34" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>23</v>
@@ -4195,10 +4195,10 @@
         <v>32</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N34" s="10" t="s">
         <v>35</v>
@@ -4207,10 +4207,10 @@
         <v>57</v>
       </c>
       <c r="P34" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R34" s="10" t="s">
         <v>51</v>
@@ -4233,28 +4233,28 @@
     </row>
     <row r="35" spans="1:23" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>312</v>
-      </c>
       <c r="G35" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>31</v>
@@ -4266,10 +4266,10 @@
         <v>32</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>35</v>
@@ -4278,10 +4278,10 @@
         <v>36</v>
       </c>
       <c r="P35" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>314</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>315</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>39</v>
@@ -4304,28 +4304,28 @@
     </row>
     <row r="36" spans="1:23" ht="30" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>318</v>
-      </c>
       <c r="G36" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>69</v>
@@ -4337,22 +4337,22 @@
         <v>32</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N36" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O36" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="P36" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="P36" s="10" t="s">
+      <c r="Q36" s="10" t="s">
         <v>321</v>
-      </c>
-      <c r="Q36" s="10" t="s">
-        <v>322</v>
       </c>
       <c r="R36" s="10" t="s">
         <v>136</v>
@@ -4375,28 +4375,28 @@
     </row>
     <row r="37" spans="1:23" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>325</v>
-      </c>
       <c r="G37" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>31</v>
@@ -4408,10 +4408,10 @@
         <v>32</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N37" s="7" t="s">
         <v>48</v>
@@ -4420,10 +4420,10 @@
         <v>36</v>
       </c>
       <c r="P37" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q37" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="Q37" s="7" t="s">
-        <v>328</v>
       </c>
       <c r="R37" s="7" t="s">
         <v>51</v>
@@ -4446,28 +4446,28 @@
     </row>
     <row r="38" spans="1:23" ht="30" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F38" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>331</v>
-      </c>
       <c r="G38" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H38" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>31</v>
@@ -4479,10 +4479,10 @@
         <v>32</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N38" s="10" t="s">
         <v>35</v>
@@ -4491,10 +4491,10 @@
         <v>36</v>
       </c>
       <c r="P38" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q38" s="10" t="s">
         <v>333</v>
-      </c>
-      <c r="Q38" s="10" t="s">
-        <v>334</v>
       </c>
       <c r="R38" s="10" t="s">
         <v>39</v>
@@ -4517,28 +4517,28 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>337</v>
-      </c>
       <c r="G39" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>293</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>23</v>
@@ -4550,7 +4550,7 @@
         <v>32</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M39" s="12" t="s">
         <v>97</v>
@@ -4562,10 +4562,10 @@
         <v>57</v>
       </c>
       <c r="P39" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q39" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="Q39" s="7" t="s">
-        <v>340</v>
       </c>
       <c r="R39" s="7" t="s">
         <v>51</v>
@@ -4588,28 +4588,28 @@
     </row>
     <row r="40" spans="1:23" ht="30" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F40" s="10" t="s">
-        <v>343</v>
-      </c>
       <c r="G40" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H40" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>23</v>
@@ -4621,10 +4621,10 @@
         <v>32</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N40" s="10" t="s">
         <v>48</v>
@@ -4633,10 +4633,10 @@
         <v>57</v>
       </c>
       <c r="P40" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q40" s="10" t="s">
         <v>345</v>
-      </c>
-      <c r="Q40" s="10" t="s">
-        <v>346</v>
       </c>
       <c r="R40" s="10" t="s">
         <v>68</v>
@@ -4659,25 +4659,25 @@
     </row>
     <row r="41" spans="1:23" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="C41" s="7" t="s">
         <v>348</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>349</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>352</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>102</v>
@@ -4692,10 +4692,10 @@
         <v>32</v>
       </c>
       <c r="L41" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>353</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>354</v>
       </c>
       <c r="N41" s="7" t="s">
         <v>35</v>
@@ -4704,10 +4704,10 @@
         <v>36</v>
       </c>
       <c r="P41" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q41" s="7" t="s">
         <v>355</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>356</v>
       </c>
       <c r="R41" s="7" t="s">
         <v>136</v>
@@ -4722,33 +4722,33 @@
         <v>42</v>
       </c>
       <c r="V41" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="W41" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="W41" s="7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="30" customHeight="1">
       <c r="A42" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="C42" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="G42" s="10" t="s">
         <v>364</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>365</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>102</v>
@@ -4763,22 +4763,22 @@
         <v>32</v>
       </c>
       <c r="L42" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="M42" s="9" t="s">
         <v>366</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>367</v>
       </c>
       <c r="N42" s="10" t="s">
         <v>35</v>
       </c>
       <c r="O42" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P42" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q42" s="10" t="s">
         <v>368</v>
-      </c>
-      <c r="Q42" s="10" t="s">
-        <v>369</v>
       </c>
       <c r="R42" s="10" t="s">
         <v>136</v>
@@ -4793,36 +4793,36 @@
         <v>42</v>
       </c>
       <c r="V42" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="W42" s="10" t="s">
         <v>370</v>
-      </c>
-      <c r="W42" s="10" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>373</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>374</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="G43" s="7" t="s">
+      <c r="H43" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>377</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>31</v>
@@ -4834,10 +4834,10 @@
         <v>32</v>
       </c>
       <c r="L43" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="M43" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="N43" s="7" t="s">
         <v>133</v>
@@ -4846,10 +4846,10 @@
         <v>36</v>
       </c>
       <c r="P43" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q43" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>381</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>51</v>
@@ -4867,30 +4867,30 @@
         <v>95</v>
       </c>
       <c r="W43" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="45" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>97</v>
       </c>
       <c r="C44" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="G44" s="10" t="s">
         <v>387</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>388</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>102</v>
@@ -4905,10 +4905,10 @@
         <v>32</v>
       </c>
       <c r="L44" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="M44" s="9" t="s">
         <v>389</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>390</v>
       </c>
       <c r="N44" s="10" t="s">
         <v>48</v>
@@ -4917,10 +4917,10 @@
         <v>57</v>
       </c>
       <c r="P44" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q44" s="10" t="s">
         <v>391</v>
-      </c>
-      <c r="Q44" s="10" t="s">
-        <v>392</v>
       </c>
       <c r="R44" s="10" t="s">
         <v>68</v>
@@ -4935,36 +4935,36 @@
         <v>42</v>
       </c>
       <c r="V44" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="W44" s="10" t="s">
         <v>393</v>
-      </c>
-      <c r="W44" s="10" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>400</v>
-      </c>
       <c r="H45" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>23</v>
@@ -4976,10 +4976,10 @@
         <v>32</v>
       </c>
       <c r="L45" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="M45" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>48</v>
@@ -4988,10 +4988,10 @@
         <v>57</v>
       </c>
       <c r="P45" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q45" s="7" t="s">
         <v>403</v>
-      </c>
-      <c r="Q45" s="7" t="s">
-        <v>404</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>39</v>
@@ -5009,30 +5009,30 @@
         <v>94</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="30" customHeight="1">
       <c r="A46" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>408</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E46" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>409</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>410</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>102</v>
@@ -5047,10 +5047,10 @@
         <v>32</v>
       </c>
       <c r="L46" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="M46" s="9" t="s">
         <v>411</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>412</v>
       </c>
       <c r="N46" s="10" t="s">
         <v>35</v>
@@ -5059,10 +5059,10 @@
         <v>57</v>
       </c>
       <c r="P46" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q46" s="10" t="s">
         <v>413</v>
-      </c>
-      <c r="Q46" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="R46" s="10" t="s">
         <v>51</v>
@@ -5077,36 +5077,36 @@
         <v>42</v>
       </c>
       <c r="V46" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="W46" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>421</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>422</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>23</v>
@@ -5118,10 +5118,10 @@
         <v>32</v>
       </c>
       <c r="L47" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>423</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>424</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>35</v>
@@ -5133,7 +5133,7 @@
         <v>149</v>
       </c>
       <c r="Q47" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>68</v>
@@ -5148,33 +5148,33 @@
         <v>42</v>
       </c>
       <c r="V47" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="W47" s="7" t="s">
         <v>426</v>
-      </c>
-      <c r="W47" s="7" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="30" customHeight="1">
       <c r="A48" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B48" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>429</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>430</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>99</v>
       </c>
       <c r="E48" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="F48" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="G48" s="10" t="s">
         <v>432</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>433</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>102</v>
@@ -5189,10 +5189,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="M48" s="9" t="s">
         <v>434</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>435</v>
       </c>
       <c r="N48" s="10" t="s">
         <v>35</v>
@@ -5201,10 +5201,10 @@
         <v>57</v>
       </c>
       <c r="P48" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q48" s="10" t="s">
         <v>436</v>
-      </c>
-      <c r="Q48" s="10" t="s">
-        <v>437</v>
       </c>
       <c r="R48" s="10" t="s">
         <v>51</v>
@@ -5219,33 +5219,33 @@
         <v>42</v>
       </c>
       <c r="V48" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="W48" s="10" t="s">
         <v>438</v>
-      </c>
-      <c r="W48" s="10" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="49" spans="1:23" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="C49" s="7" t="s">
         <v>441</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>442</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E49" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="G49" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>445</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>102</v>
@@ -5260,10 +5260,10 @@
         <v>32</v>
       </c>
       <c r="L49" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="M49" s="6" t="s">
         <v>446</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>447</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>35</v>
@@ -5272,10 +5272,10 @@
         <v>57</v>
       </c>
       <c r="P49" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q49" s="7" t="s">
         <v>448</v>
-      </c>
-      <c r="Q49" s="7" t="s">
-        <v>449</v>
       </c>
       <c r="R49" s="7" t="s">
         <v>136</v>
@@ -5290,10 +5290,10 @@
         <v>42</v>
       </c>
       <c r="V49" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="W49" s="7" t="s">
         <v>450</v>
-      </c>
-      <c r="W49" s="7" t="s">
-        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -5344,7 +5344,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5369,13 +5369,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>454</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F2" s="3">
         <v>48</v>
@@ -5383,41 +5383,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>456</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>458</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>466</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>460</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5425,13 +5425,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>462</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F6" s="3">
         <v>105</v>
@@ -5513,22 +5513,22 @@
         <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>470</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>471</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>473</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>474</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>102</v>
@@ -5537,16 +5537,16 @@
         <v>31</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>478</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>35</v>
@@ -5555,10 +5555,10 @@
         <v>36</v>
       </c>
       <c r="P9" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>479</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>480</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>39</v>
@@ -5570,13 +5570,13 @@
         <v>41</v>
       </c>
       <c r="U9" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="V9" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="W9" s="7" t="s">
         <v>482</v>
-      </c>
-      <c r="W9" s="7" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -5584,34 +5584,34 @@
         <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>484</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>485</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>179</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>488</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>489</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>476</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>117</v>
@@ -5626,10 +5626,10 @@
         <v>36</v>
       </c>
       <c r="P10" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q10" s="10" t="s">
         <v>490</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>491</v>
       </c>
       <c r="R10" s="10" t="s">
         <v>51</v>
@@ -5641,13 +5641,13 @@
         <v>187</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="30" customHeight="1">
@@ -5655,37 +5655,37 @@
         <v>52</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>484</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>485</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>179</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>495</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>476</v>
-      </c>
       <c r="L11" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>496</v>
@@ -5706,13 +5706,13 @@
         <v>136</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T11" s="7" t="s">
         <v>187</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>500</v>
@@ -5750,10 +5750,10 @@
         <v>23</v>
       </c>
       <c r="J12" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>476</v>
       </c>
       <c r="L12" s="11" t="s">
         <v>117</v>
@@ -5783,7 +5783,7 @@
         <v>187</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V12" s="10" t="s">
         <v>189</v>
@@ -5821,10 +5821,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>475</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>476</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>516</v>
@@ -5854,7 +5854,7 @@
         <v>187</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>520</v>
@@ -5868,10 +5868,10 @@
         <v>75</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>26</v>
@@ -5883,19 +5883,19 @@
         <v>523</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>293</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="K14" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>476</v>
       </c>
       <c r="L14" s="11" t="s">
         <v>117</v>
@@ -5925,7 +5925,7 @@
         <v>41</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V14" s="10" t="s">
         <v>120</v>
@@ -5939,13 +5939,13 @@
         <v>83</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>362</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>526</v>
@@ -5963,10 +5963,10 @@
         <v>31</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>475</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>476</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>530</v>
@@ -5996,13 +5996,13 @@
         <v>41</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="V15" s="7" t="s">
         <v>534</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@278eae0a01380232729710afaa9a20d9171ea92a 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -511,904 +511,904 @@
     <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
   </si>
   <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
+  </si>
+  <si>
+    <t>/LEDs</t>
+  </si>
+  <si>
+    <t>87.9944</t>
+  </si>
+  <si>
+    <t>10.4000</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>JST PH 4</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
+    <t>127.8644</t>
+  </si>
+  <si>
+    <t>77.1844</t>
+  </si>
+  <si>
+    <t>12.4000</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>Connector_Audio</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>71.9889</t>
+  </si>
+  <si>
+    <t>106.4944</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>11.2000</t>
+  </si>
+  <si>
+    <t>6.7000</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J8 J18 J19 J20 J22</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(6)</t>
+  </si>
+  <si>
+    <t>157.6094</t>
+  </si>
+  <si>
+    <t>97.1944</t>
+  </si>
+  <si>
+    <t>15.7000</t>
+  </si>
+  <si>
+    <t>19.2300</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>Pedalboard Soundcard</t>
+  </si>
+  <si>
+    <t>Pedalboard_Soundcard</t>
+  </si>
+  <si>
+    <t>102.2444</t>
+  </si>
+  <si>
+    <t>62.6188</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>41.4500</t>
+  </si>
+  <si>
+    <t>55.0150</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
+  </si>
+  <si>
+    <t>160.4944</t>
+  </si>
+  <si>
+    <t>102.7844</t>
+  </si>
+  <si>
+    <t>7.6000</t>
+  </si>
+  <si>
+    <t>2.6000</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>Inductor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(4)</t>
+  </si>
+  <si>
+    <t>61.5944</t>
+  </si>
+  <si>
+    <t>90.0944</t>
+  </si>
+  <si>
+    <t>2.4500</t>
+  </si>
+  <si>
+    <t>0.9500</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>pspice</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
+    <t>146.8944</t>
+  </si>
+  <si>
+    <t>80.8544</t>
+  </si>
+  <si>
+    <t>5.1000</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+  </si>
+  <si>
+    <t>141.8544</t>
+  </si>
+  <si>
+    <t>102.8344</t>
+  </si>
+  <si>
+    <t>4.4150</t>
+  </si>
+  <si>
+    <t>7.4000</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R5 R13</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>Resistor_SMD</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>60.7244</t>
+  </si>
+  <si>
+    <t>76.1544</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>R6 R10</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+  </si>
+  <si>
+    <t>81.3944</t>
+  </si>
+  <si>
+    <t>84.6344</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+  </si>
+  <si>
+    <t>62.6244</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>R3 R7 R20</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(3)</t>
+  </si>
+  <si>
+    <t>64.0194</t>
+  </si>
+  <si>
+    <t>89.5694</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>R1 R2 R8 R11 R16</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>pedalboard-hw(5)</t>
+  </si>
+  <si>
+    <t>153.0944</t>
+  </si>
+  <si>
+    <t>100.1644</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>R15 R17</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
+  </si>
+  <si>
+    <t>137.8244</t>
+  </si>
+  <si>
+    <t>87.2244</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>R18 R19</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
+  </si>
+  <si>
+    <t>130.7344</t>
+  </si>
+  <si>
+    <t>86.1844</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
+  </si>
+  <si>
+    <t>135.9044</t>
+  </si>
+  <si>
+    <t>83.8644</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
+  </si>
+  <si>
+    <t>140.6644</t>
+  </si>
+  <si>
+    <t>81.1944</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>42.2444</t>
+  </si>
+  <si>
+    <t>99.4944</t>
+  </si>
+  <si>
+    <t>16.5000</t>
+  </si>
+  <si>
+    <t>14.4000</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>11.9944</t>
+  </si>
+  <si>
+    <t>63.9944</t>
+  </si>
+  <si>
+    <t>16.0000</t>
+  </si>
+  <si>
+    <t>6.8000</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U1 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+  </si>
+  <si>
+    <t>70.4544</t>
+  </si>
+  <si>
+    <t>78.6444</t>
+  </si>
+  <si>
+    <t>1.7000</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>CM4IO</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+  </si>
+  <si>
+    <t>141.5144</t>
+  </si>
+  <si>
+    <t>88.5944</t>
+  </si>
+  <si>
+    <t>6.9000</t>
+  </si>
+  <si>
+    <t>4.9000</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>Regulator_Linear</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>115.1644</t>
+  </si>
+  <si>
+    <t>74.1444</t>
+  </si>
+  <si>
+    <t>6.1000</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+  </si>
+  <si>
+    <t>89.3944</t>
+  </si>
+  <si>
+    <t>85.3944</t>
+  </si>
+  <si>
+    <t>7.7500</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>Isolator</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>Package_SO</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>65.7444</t>
+  </si>
+  <si>
+    <t>80.6544</t>
+  </si>
+  <si>
+    <t>10.8000</t>
+  </si>
+  <si>
+    <t>3.3400</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
+  </si>
+  <si>
+    <t>81.4944</t>
+  </si>
+  <si>
+    <t>78.5444</t>
+  </si>
+  <si>
+    <t>8.8000</t>
+  </si>
+  <si>
+    <t>4.4100</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABLS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
+  </si>
+  <si>
+    <t>99.9944</t>
+  </si>
+  <si>
+    <t>74.8944</t>
+  </si>
+  <si>
+    <t>14.6000</t>
+  </si>
+  <si>
+    <t>2.1000</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-hw</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>4.0.0-RC1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-12-05</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>8.0.4+1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>106 (85 SMD/ 20 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>95 (82 SMD/ 12 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_Switch</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Barrel_Jack_MountingPin</t>
+  </si>
+  <si>
+    <t>BarrelJack_Wuerth_6941xx301002</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
+  </si>
+  <si>
+    <t>161.3944</t>
+  </si>
+  <si>
+    <t>100.5944</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>7.9000</t>
+  </si>
+  <si>
+    <t>DIN-5_180degree</t>
+  </si>
+  <si>
+    <t>J2 J4</t>
+  </si>
+  <si>
+    <t>DIN5</t>
+  </si>
+  <si>
+    <t>CP-2350</t>
+  </si>
+  <si>
+    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
+  </si>
+  <si>
+    <t>71.9944</t>
+  </si>
+  <si>
+    <t>108.9944</t>
+  </si>
+  <si>
+    <t>17.5000</t>
+  </si>
+  <si>
+    <t>14.7500</t>
+  </si>
+  <si>
+    <t>J12 J16</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm</t>
+  </si>
+  <si>
+    <t>111.3094</t>
+  </si>
+  <si>
+    <t>86.5444</t>
+  </si>
+  <si>
+    <t>6.7800</t>
+  </si>
+  <si>
+    <t>J25 J26</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
+  </si>
+  <si>
     <t>Connector_JST</t>
-  </si>
-  <si>
-    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
-  </si>
-  <si>
-    <t>/LEDs</t>
-  </si>
-  <si>
-    <t>87.9944</t>
-  </si>
-  <si>
-    <t>10.4000</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>JST PH 4</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
-  </si>
-  <si>
-    <t>127.8644</t>
-  </si>
-  <si>
-    <t>77.1844</t>
-  </si>
-  <si>
-    <t>12.4000</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>Connector_Audio</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>71.9889</t>
-  </si>
-  <si>
-    <t>106.4944</t>
-  </si>
-  <si>
-    <t>THT</t>
-  </si>
-  <si>
-    <t>11.2000</t>
-  </si>
-  <si>
-    <t>6.7000</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J8 J18 J19 J20 J22</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(6)</t>
-  </si>
-  <si>
-    <t>157.6094</t>
-  </si>
-  <si>
-    <t>97.1944</t>
-  </si>
-  <si>
-    <t>15.7000</t>
-  </si>
-  <si>
-    <t>19.2300</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Raspberry_Sound_Card</t>
-  </si>
-  <si>
-    <t>J27</t>
-  </si>
-  <si>
-    <t>Pedalboard Soundcard</t>
-  </si>
-  <si>
-    <t>Pedalboard_Soundcard</t>
-  </si>
-  <si>
-    <t>102.2444</t>
-  </si>
-  <si>
-    <t>62.6188</t>
-  </si>
-  <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>41.4500</t>
-  </si>
-  <si>
-    <t>55.0150</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
-  </si>
-  <si>
-    <t>TerminalBlock_Phoenix</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
-  </si>
-  <si>
-    <t>160.4944</t>
-  </si>
-  <si>
-    <t>102.7844</t>
-  </si>
-  <si>
-    <t>7.6000</t>
-  </si>
-  <si>
-    <t>2.6000</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>Inductor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(4)</t>
-  </si>
-  <si>
-    <t>61.5944</t>
-  </si>
-  <si>
-    <t>90.0944</t>
-  </si>
-  <si>
-    <t>2.4500</t>
-  </si>
-  <si>
-    <t>0.9500</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>pspice</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
-  </si>
-  <si>
-    <t>146.8944</t>
-  </si>
-  <si>
-    <t>80.8544</t>
-  </si>
-  <si>
-    <t>5.1000</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
-  </si>
-  <si>
-    <t>141.8544</t>
-  </si>
-  <si>
-    <t>102.8344</t>
-  </si>
-  <si>
-    <t>4.4150</t>
-  </si>
-  <si>
-    <t>7.4000</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R5 R13</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>Resistor_SMD</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>60.7244</t>
-  </si>
-  <si>
-    <t>76.1544</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>R6 R10</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
-  </si>
-  <si>
-    <t>81.3944</t>
-  </si>
-  <si>
-    <t>84.6344</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
-  </si>
-  <si>
-    <t>62.6244</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>R3 R7 R20</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(3)</t>
-  </si>
-  <si>
-    <t>64.0194</t>
-  </si>
-  <si>
-    <t>89.5694</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>R1 R2 R8 R11 R16</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>pedalboard-hw(5)</t>
-  </si>
-  <si>
-    <t>153.0944</t>
-  </si>
-  <si>
-    <t>100.1644</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>R15 R17</t>
-  </si>
-  <si>
-    <t>2K2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345</t>
-  </si>
-  <si>
-    <t>137.8244</t>
-  </si>
-  <si>
-    <t>87.2244</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R18 R19</t>
-  </si>
-  <si>
-    <t>3K9</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
-  </si>
-  <si>
-    <t>130.7344</t>
-  </si>
-  <si>
-    <t>86.1844</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>12K</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
-  </si>
-  <si>
-    <t>135.9044</t>
-  </si>
-  <si>
-    <t>83.8644</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
-  </si>
-  <si>
-    <t>140.6644</t>
-  </si>
-  <si>
-    <t>81.1944</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>42.2444</t>
-  </si>
-  <si>
-    <t>99.4944</t>
-  </si>
-  <si>
-    <t>16.5000</t>
-  </si>
-  <si>
-    <t>14.4000</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
-  </si>
-  <si>
-    <t>Tactile Button</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>11.9944</t>
-  </si>
-  <si>
-    <t>63.9944</t>
-  </si>
-  <si>
-    <t>16.0000</t>
-  </si>
-  <si>
-    <t>6.8000</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U1 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
-  </si>
-  <si>
-    <t>70.4544</t>
-  </si>
-  <si>
-    <t>78.6444</t>
-  </si>
-  <si>
-    <t>1.7000</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>CM4IO</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
-  </si>
-  <si>
-    <t>141.5144</t>
-  </si>
-  <si>
-    <t>88.5944</t>
-  </si>
-  <si>
-    <t>6.9000</t>
-  </si>
-  <si>
-    <t>4.9000</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>Regulator_Linear</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
-  </si>
-  <si>
-    <t>115.1644</t>
-  </si>
-  <si>
-    <t>74.1444</t>
-  </si>
-  <si>
-    <t>6.1000</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
-  </si>
-  <si>
-    <t>89.3944</t>
-  </si>
-  <si>
-    <t>85.3944</t>
-  </si>
-  <si>
-    <t>7.7500</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>Isolator</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>Package_SO</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>65.7444</t>
-  </si>
-  <si>
-    <t>80.6544</t>
-  </si>
-  <si>
-    <t>10.8000</t>
-  </si>
-  <si>
-    <t>3.3400</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>81.4944</t>
-  </si>
-  <si>
-    <t>78.5444</t>
-  </si>
-  <si>
-    <t>8.8000</t>
-  </si>
-  <si>
-    <t>4.4100</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABLS-12.000MHZ-B4-T</t>
-  </si>
-  <si>
-    <t>Crystal_SMD_HC49-US</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Resonators/ABLS.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ABLS-12-000MHZ-B4-T/2184161</t>
-  </si>
-  <si>
-    <t>99.9944</t>
-  </si>
-  <si>
-    <t>74.8944</t>
-  </si>
-  <si>
-    <t>14.6000</t>
-  </si>
-  <si>
-    <t>2.1000</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-hw</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>4.0.0-RC1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-12-05</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>8.0.4+1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>106 (85 SMD/ 20 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>95 (82 SMD/ 12 THT)</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_Switch</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Barrel_Jack_MountingPin</t>
-  </si>
-  <si>
-    <t>BarrelJack_Wuerth_6941xx301002</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (DNF)</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6941xx301002.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
-  </si>
-  <si>
-    <t>161.3944</t>
-  </si>
-  <si>
-    <t>100.5944</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>7.9000</t>
-  </si>
-  <si>
-    <t>DIN-5_180degree</t>
-  </si>
-  <si>
-    <t>J2 J4</t>
-  </si>
-  <si>
-    <t>DIN5</t>
-  </si>
-  <si>
-    <t>CP-2350</t>
-  </si>
-  <si>
-    <t>https://www.switchcraft.com/assets/1/24/57PC5F_CD.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
-  </si>
-  <si>
-    <t>71.9944</t>
-  </si>
-  <si>
-    <t>108.9944</t>
-  </si>
-  <si>
-    <t>17.5000</t>
-  </si>
-  <si>
-    <t>14.7500</t>
-  </si>
-  <si>
-    <t>J12 J16</t>
-  </si>
-  <si>
-    <t>Debug</t>
-  </si>
-  <si>
-    <t>PinHeader_1x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>Connector_PinHeader_2.54mm</t>
-  </si>
-  <si>
-    <t>111.3094</t>
-  </si>
-  <si>
-    <t>86.5444</t>
-  </si>
-  <si>
-    <t>6.7800</t>
-  </si>
-  <si>
-    <t>J25 J26</t>
-  </si>
-  <si>
-    <t>JST_PH_B3B-PH-K_1x03_P2.00mm_Vertical</t>
   </si>
   <si>
     <t>54.9544</t>
@@ -2089,7 +2089,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2114,13 +2114,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>416</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -2128,41 +2128,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>418</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>422</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2170,13 +2170,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>424</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F6" s="3">
         <v>95</v>
@@ -3199,7 +3199,7 @@
         <v>162</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>163</v>
+        <v>100</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>23</v>
@@ -3211,13 +3211,13 @@
         <v>32</v>
       </c>
       <c r="L22" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="M22" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="M22" s="12" t="s">
+      <c r="N22" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="N22" s="11" t="s">
-        <v>166</v>
       </c>
       <c r="O22" s="9" t="s">
         <v>57</v>
@@ -3226,7 +3226,7 @@
         <v>142</v>
       </c>
       <c r="Q22" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R22" s="11" t="s">
         <v>51</v>
@@ -3241,7 +3241,7 @@
         <v>42</v>
       </c>
       <c r="V22" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="W22" s="11" t="s">
         <v>143</v>
@@ -3255,19 +3255,19 @@
         <v>24</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>159</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>100</v>
@@ -3282,10 +3282,10 @@
         <v>32</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N23" s="7" t="s">
         <v>35</v>
@@ -3294,10 +3294,10 @@
         <v>57</v>
       </c>
       <c r="P23" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>51</v>
@@ -3312,7 +3312,7 @@
         <v>42</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W23" s="7" t="s">
         <v>143</v>
@@ -3320,25 +3320,25 @@
     </row>
     <row r="24" spans="1:23" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>100</v>
@@ -3353,10 +3353,10 @@
         <v>32</v>
       </c>
       <c r="L24" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="M24" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>184</v>
       </c>
       <c r="N24" s="11" t="s">
         <v>35</v>
@@ -3365,10 +3365,10 @@
         <v>36</v>
       </c>
       <c r="P24" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q24" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="Q24" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="R24" s="11" t="s">
         <v>39</v>
@@ -3377,39 +3377,39 @@
         <v>40</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V24" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="W24" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="W24" s="11" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>194</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>100</v>
@@ -3424,22 +3424,22 @@
         <v>32</v>
       </c>
       <c r="L25" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="M25" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>196</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="P25" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="P25" s="7" t="s">
+      <c r="Q25" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="Q25" s="7" t="s">
-        <v>199</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>106</v>
@@ -3448,39 +3448,39 @@
         <v>40</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U25" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V25" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="W25" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:23">
       <c r="A26" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>206</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>100</v>
@@ -3507,54 +3507,54 @@
         <v>57</v>
       </c>
       <c r="P26" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q26" s="11" t="s">
         <v>207</v>
-      </c>
-      <c r="Q26" s="11" t="s">
-        <v>208</v>
       </c>
       <c r="R26" s="11" t="s">
         <v>39</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U26" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V26" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="W26" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="W26" s="11" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>159</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>23</v>
@@ -3569,7 +3569,7 @@
         <v>113</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>48</v>
@@ -3578,10 +3578,10 @@
         <v>57</v>
       </c>
       <c r="P27" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q27" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>51</v>
@@ -3590,42 +3590,42 @@
         <v>40</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>42</v>
       </c>
       <c r="V27" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="W27" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="W27" s="7" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="H28" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>227</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>60</v>
@@ -3637,22 +3637,22 @@
         <v>32</v>
       </c>
       <c r="L28" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="M28" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>229</v>
       </c>
       <c r="N28" s="11" t="s">
         <v>35</v>
       </c>
       <c r="O28" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="P28" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="P28" s="11" t="s">
+      <c r="Q28" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="Q28" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="R28" s="11" t="s">
         <v>68</v>
@@ -3667,36 +3667,36 @@
         <v>42</v>
       </c>
       <c r="V28" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="W28" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="W28" s="11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="H29" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>23</v>
@@ -3708,10 +3708,10 @@
         <v>32</v>
       </c>
       <c r="L29" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="M29" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="M29" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>48</v>
@@ -3720,10 +3720,10 @@
         <v>57</v>
       </c>
       <c r="P29" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>68</v>
@@ -3741,30 +3741,30 @@
         <v>143</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E30" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>248</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>249</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>100</v>
@@ -3779,10 +3779,10 @@
         <v>32</v>
       </c>
       <c r="L30" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="M30" s="12" t="s">
         <v>250</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>251</v>
       </c>
       <c r="N30" s="11" t="s">
         <v>48</v>
@@ -3791,10 +3791,10 @@
         <v>57</v>
       </c>
       <c r="P30" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q30" s="11" t="s">
         <v>252</v>
-      </c>
-      <c r="Q30" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="R30" s="11" t="s">
         <v>106</v>
@@ -3809,36 +3809,36 @@
         <v>42</v>
       </c>
       <c r="V30" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="W30" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="W30" s="11" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>31</v>
@@ -3850,10 +3850,10 @@
         <v>32</v>
       </c>
       <c r="L31" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="M31" s="8" t="s">
         <v>262</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>35</v>
@@ -3862,10 +3862,10 @@
         <v>36</v>
       </c>
       <c r="P31" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q31" s="7" t="s">
         <v>264</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>68</v>
@@ -3888,28 +3888,28 @@
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>268</v>
-      </c>
       <c r="G32" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>31</v>
@@ -3921,10 +3921,10 @@
         <v>32</v>
       </c>
       <c r="L32" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="M32" s="12" t="s">
         <v>269</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>270</v>
       </c>
       <c r="N32" s="11" t="s">
         <v>35</v>
@@ -3933,10 +3933,10 @@
         <v>36</v>
       </c>
       <c r="P32" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q32" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="Q32" s="11" t="s">
-        <v>272</v>
       </c>
       <c r="R32" s="11" t="s">
         <v>106</v>
@@ -3959,28 +3959,28 @@
     </row>
     <row r="33" spans="1:23" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>275</v>
-      </c>
       <c r="G33" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>23</v>
@@ -3992,10 +3992,10 @@
         <v>32</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N33" s="7" t="s">
         <v>35</v>
@@ -4004,10 +4004,10 @@
         <v>57</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>51</v>
@@ -4030,28 +4030,28 @@
     </row>
     <row r="34" spans="1:23" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F34" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>280</v>
-      </c>
       <c r="G34" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H34" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>52</v>
@@ -4063,22 +4063,22 @@
         <v>32</v>
       </c>
       <c r="L34" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M34" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N34" s="11" t="s">
         <v>35</v>
       </c>
       <c r="O34" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="P34" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="P34" s="11" t="s">
+      <c r="Q34" s="11" t="s">
         <v>283</v>
-      </c>
-      <c r="Q34" s="11" t="s">
-        <v>284</v>
       </c>
       <c r="R34" s="11" t="s">
         <v>106</v>
@@ -4101,28 +4101,28 @@
     </row>
     <row r="35" spans="1:23" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>287</v>
-      </c>
       <c r="G35" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H35" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>69</v>
@@ -4134,22 +4134,22 @@
         <v>32</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N35" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O35" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="P35" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="P35" s="7" t="s">
+      <c r="Q35" s="7" t="s">
         <v>290</v>
-      </c>
-      <c r="Q35" s="7" t="s">
-        <v>291</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>106</v>
@@ -4172,28 +4172,28 @@
     </row>
     <row r="36" spans="1:23" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>294</v>
-      </c>
       <c r="G36" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="I36" s="9" t="s">
         <v>31</v>
@@ -4205,10 +4205,10 @@
         <v>32</v>
       </c>
       <c r="L36" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M36" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N36" s="11" t="s">
         <v>48</v>
@@ -4217,10 +4217,10 @@
         <v>36</v>
       </c>
       <c r="P36" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q36" s="11" t="s">
         <v>296</v>
-      </c>
-      <c r="Q36" s="11" t="s">
-        <v>297</v>
       </c>
       <c r="R36" s="11" t="s">
         <v>51</v>
@@ -4243,28 +4243,28 @@
     </row>
     <row r="37" spans="1:23" ht="30" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>300</v>
-      </c>
       <c r="G37" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>31</v>
@@ -4276,10 +4276,10 @@
         <v>32</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N37" s="7" t="s">
         <v>35</v>
@@ -4288,10 +4288,10 @@
         <v>36</v>
       </c>
       <c r="P37" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q37" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="Q37" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="R37" s="7" t="s">
         <v>39</v>
@@ -4314,28 +4314,28 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="F38" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>306</v>
-      </c>
       <c r="G38" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="I38" s="9" t="s">
         <v>23</v>
@@ -4347,7 +4347,7 @@
         <v>32</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M38" s="10" t="s">
         <v>24</v>
@@ -4359,10 +4359,10 @@
         <v>57</v>
       </c>
       <c r="P38" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q38" s="11" t="s">
         <v>308</v>
-      </c>
-      <c r="Q38" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="R38" s="11" t="s">
         <v>51</v>
@@ -4385,28 +4385,28 @@
     </row>
     <row r="39" spans="1:23" ht="30" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>312</v>
-      </c>
       <c r="G39" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>23</v>
@@ -4418,10 +4418,10 @@
         <v>32</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="N39" s="7" t="s">
         <v>48</v>
@@ -4430,10 +4430,10 @@
         <v>57</v>
       </c>
       <c r="P39" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q39" s="7" t="s">
         <v>314</v>
-      </c>
-      <c r="Q39" s="7" t="s">
-        <v>315</v>
       </c>
       <c r="R39" s="7" t="s">
         <v>68</v>
@@ -4456,25 +4456,25 @@
     </row>
     <row r="40" spans="1:23" ht="30" customHeight="1">
       <c r="A40" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E40" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>319</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>320</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>100</v>
@@ -4489,10 +4489,10 @@
         <v>32</v>
       </c>
       <c r="L40" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="M40" s="12" t="s">
         <v>321</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>322</v>
       </c>
       <c r="N40" s="11" t="s">
         <v>35</v>
@@ -4501,10 +4501,10 @@
         <v>36</v>
       </c>
       <c r="P40" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q40" s="11" t="s">
         <v>323</v>
-      </c>
-      <c r="Q40" s="11" t="s">
-        <v>324</v>
       </c>
       <c r="R40" s="11" t="s">
         <v>106</v>
@@ -4513,39 +4513,39 @@
         <v>40</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U40" s="11" t="s">
         <v>42</v>
       </c>
       <c r="V40" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="W40" s="11" t="s">
         <v>325</v>
-      </c>
-      <c r="W40" s="11" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>331</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>332</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>100</v>
@@ -4560,22 +4560,22 @@
         <v>32</v>
       </c>
       <c r="L41" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="M41" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="M41" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="N41" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P41" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q41" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>336</v>
       </c>
       <c r="R41" s="7" t="s">
         <v>106</v>
@@ -4590,36 +4590,36 @@
         <v>42</v>
       </c>
       <c r="V41" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="W41" s="7" t="s">
         <v>337</v>
-      </c>
-      <c r="W41" s="7" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="30" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E42" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>341</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="G42" s="11" t="s">
+      <c r="H42" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>343</v>
       </c>
       <c r="I42" s="9" t="s">
         <v>31</v>
@@ -4631,22 +4631,22 @@
         <v>32</v>
       </c>
       <c r="L42" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="M42" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="M42" s="12" t="s">
-        <v>345</v>
-      </c>
       <c r="N42" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O42" s="9" t="s">
         <v>36</v>
       </c>
       <c r="P42" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q42" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="Q42" s="11" t="s">
-        <v>347</v>
       </c>
       <c r="R42" s="11" t="s">
         <v>51</v>
@@ -4664,30 +4664,30 @@
         <v>94</v>
       </c>
       <c r="W42" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="45" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>353</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>354</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>100</v>
@@ -4702,10 +4702,10 @@
         <v>32</v>
       </c>
       <c r="L43" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="M43" s="8" t="s">
         <v>355</v>
-      </c>
-      <c r="M43" s="8" t="s">
-        <v>356</v>
       </c>
       <c r="N43" s="7" t="s">
         <v>48</v>
@@ -4714,10 +4714,10 @@
         <v>57</v>
       </c>
       <c r="P43" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q43" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>358</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>68</v>
@@ -4732,36 +4732,36 @@
         <v>42</v>
       </c>
       <c r="V43" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="W43" s="7" t="s">
         <v>359</v>
-      </c>
-      <c r="W43" s="7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="30" customHeight="1">
       <c r="A44" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C44" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="E44" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="F44" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="G44" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>365</v>
-      </c>
       <c r="H44" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>23</v>
@@ -4773,10 +4773,10 @@
         <v>32</v>
       </c>
       <c r="L44" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="M44" s="12" t="s">
         <v>366</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>367</v>
       </c>
       <c r="N44" s="11" t="s">
         <v>48</v>
@@ -4785,10 +4785,10 @@
         <v>57</v>
       </c>
       <c r="P44" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q44" s="11" t="s">
         <v>368</v>
-      </c>
-      <c r="Q44" s="11" t="s">
-        <v>369</v>
       </c>
       <c r="R44" s="11" t="s">
         <v>39</v>
@@ -4806,30 +4806,30 @@
         <v>93</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="1:23" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>97</v>
       </c>
       <c r="E45" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>373</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>374</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>100</v>
@@ -4844,10 +4844,10 @@
         <v>32</v>
       </c>
       <c r="L45" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="M45" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="M45" s="8" t="s">
-        <v>376</v>
       </c>
       <c r="N45" s="7" t="s">
         <v>35</v>
@@ -4856,10 +4856,10 @@
         <v>57</v>
       </c>
       <c r="P45" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q45" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="Q45" s="7" t="s">
-        <v>378</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>51</v>
@@ -4874,36 +4874,36 @@
         <v>42</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="W45" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:23" ht="30" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="E46" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="F46" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="G46" s="11" t="s">
+      <c r="H46" s="11" t="s">
         <v>384</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>385</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>23</v>
@@ -4915,10 +4915,10 @@
         <v>32</v>
       </c>
       <c r="L46" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="M46" s="12" t="s">
         <v>386</v>
-      </c>
-      <c r="M46" s="12" t="s">
-        <v>387</v>
       </c>
       <c r="N46" s="11" t="s">
         <v>35</v>
@@ -4927,10 +4927,10 @@
         <v>57</v>
       </c>
       <c r="P46" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q46" s="11" t="s">
         <v>388</v>
-      </c>
-      <c r="Q46" s="11" t="s">
-        <v>389</v>
       </c>
       <c r="R46" s="11" t="s">
         <v>68</v>
@@ -4945,33 +4945,33 @@
         <v>42</v>
       </c>
       <c r="V46" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="W46" s="11" t="s">
         <v>390</v>
-      </c>
-      <c r="W46" s="11" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="47" spans="1:23" ht="30" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>97</v>
       </c>
       <c r="E47" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>395</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>396</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>100</v>
@@ -4986,10 +4986,10 @@
         <v>32</v>
       </c>
       <c r="L47" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="M47" s="8" t="s">
         <v>397</v>
-      </c>
-      <c r="M47" s="8" t="s">
-        <v>398</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>35</v>
@@ -4998,10 +4998,10 @@
         <v>57</v>
       </c>
       <c r="P47" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q47" s="7" t="s">
         <v>399</v>
-      </c>
-      <c r="Q47" s="7" t="s">
-        <v>400</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>51</v>
@@ -5016,33 +5016,33 @@
         <v>42</v>
       </c>
       <c r="V47" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="W47" s="7" t="s">
         <v>401</v>
-      </c>
-      <c r="W47" s="7" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E48" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>407</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>100</v>
@@ -5057,10 +5057,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="M48" s="12" t="s">
         <v>408</v>
-      </c>
-      <c r="M48" s="12" t="s">
-        <v>409</v>
       </c>
       <c r="N48" s="11" t="s">
         <v>35</v>
@@ -5069,10 +5069,10 @@
         <v>57</v>
       </c>
       <c r="P48" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="Q48" s="11" t="s">
         <v>410</v>
-      </c>
-      <c r="Q48" s="11" t="s">
-        <v>411</v>
       </c>
       <c r="R48" s="11" t="s">
         <v>106</v>
@@ -5087,10 +5087,10 @@
         <v>42</v>
       </c>
       <c r="V48" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="W48" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="W48" s="11" t="s">
-        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5141,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -5166,13 +5166,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>416</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F2" s="3">
         <v>47</v>
@@ -5180,41 +5180,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>418</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>422</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -5222,13 +5222,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>424</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F6" s="3">
         <v>95</v>
@@ -5313,19 +5313,19 @@
         <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>159</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>434</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>435</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>100</v>
@@ -5334,16 +5334,16 @@
         <v>23</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>439</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>48</v>
@@ -5352,10 +5352,10 @@
         <v>57</v>
       </c>
       <c r="P9" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>440</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>441</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>39</v>
@@ -5364,16 +5364,16 @@
         <v>40</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U9" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="V9" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="V9" s="7" t="s">
-        <v>443</v>
-      </c>
       <c r="W9" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="30" customHeight="1">
@@ -5384,19 +5384,19 @@
         <v>24</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>159</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>446</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>447</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>100</v>
@@ -5405,16 +5405,16 @@
         <v>31</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>437</v>
-      </c>
       <c r="L10" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="M10" s="12" t="s">
         <v>448</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>449</v>
       </c>
       <c r="N10" s="11" t="s">
         <v>35</v>
@@ -5423,10 +5423,10 @@
         <v>36</v>
       </c>
       <c r="P10" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q10" s="11" t="s">
         <v>450</v>
-      </c>
-      <c r="Q10" s="11" t="s">
-        <v>451</v>
       </c>
       <c r="R10" s="11" t="s">
         <v>39</v>
@@ -5435,16 +5435,16 @@
         <v>40</v>
       </c>
       <c r="T10" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V10" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="W10" s="11" t="s">
         <v>452</v>
-      </c>
-      <c r="W10" s="11" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -5461,25 +5461,25 @@
         <v>159</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>456</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>457</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>113</v>
@@ -5494,10 +5494,10 @@
         <v>36</v>
       </c>
       <c r="P11" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>458</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>459</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>51</v>
@@ -5506,16 +5506,16 @@
         <v>40</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="30" customHeight="1">
@@ -5532,31 +5532,31 @@
         <v>159</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>161</v>
       </c>
       <c r="G12" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>462</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>437</v>
-      </c>
       <c r="L12" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="N12" s="11" t="s">
         <v>35</v>
@@ -5574,13 +5574,13 @@
         <v>106</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V12" s="11" t="s">
         <v>465</v>
@@ -5618,10 +5618,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>471</v>
@@ -5648,10 +5648,10 @@
         <v>40</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>475</v>
@@ -5668,7 +5668,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>26</v>
@@ -5680,19 +5680,19 @@
         <v>478</v>
       </c>
       <c r="G14" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>261</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>437</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>113</v>
@@ -5722,7 +5722,7 @@
         <v>41</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V14" s="11" t="s">
         <v>116</v>
@@ -5739,10 +5739,10 @@
         <v>24</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>328</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>329</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>481</v>
@@ -5760,10 +5760,10 @@
         <v>31</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>436</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>485</v>
@@ -5793,13 +5793,13 @@
         <v>41</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="V15" s="7" t="s">
         <v>489</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@ec2cf5a4450f57a3e93c2f13b006314181f0e247 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -511,10 +511,10 @@
     <t>/LEDs</t>
   </si>
   <si>
-    <t>73.8944</t>
-  </si>
-  <si>
-    <t>87.9944</t>
+    <t>119.2944</t>
+  </si>
+  <si>
+    <t>78.1944</t>
   </si>
   <si>
     <t>10.4000</t>
@@ -1123,10 +1123,10 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
-    <t>70.4544</t>
-  </si>
-  <si>
-    <t>78.6444</t>
+    <t>121.7444</t>
+  </si>
+  <si>
+    <t>87.4944</t>
   </si>
   <si>
     <t>1.7000</t>
@@ -5003,7 +5003,7 @@
         <v>368</v>
       </c>
       <c r="R45" s="7" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="S45" s="7" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@a383db0b299569287ab8f50cb4ba9c92fdaf1c21 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -313,10 +313,10 @@
     <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
   </si>
   <si>
-    <t>135.2644</t>
-  </si>
-  <si>
-    <t>75.8644</t>
+    <t>136.7734</t>
+  </si>
+  <si>
+    <t>73.5802</t>
   </si>
   <si>
     <t>8.3000</t>
@@ -436,10 +436,10 @@
     <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
   </si>
   <si>
-    <t>63.0944</t>
-  </si>
-  <si>
-    <t>87.4544</t>
+    <t>65.6560</t>
+  </si>
+  <si>
+    <t>89.0730</t>
   </si>
   <si>
     <t>3.9000</t>
@@ -763,10 +763,10 @@
     <t>pedalboard-hw(4)</t>
   </si>
   <si>
-    <t>61.5944</t>
-  </si>
-  <si>
-    <t>90.0944</t>
+    <t>63.0160</t>
+  </si>
+  <si>
+    <t>87.5730</t>
   </si>
   <si>
     <t>2.4500</t>
@@ -862,10 +862,10 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
-    <t>60.7244</t>
-  </si>
-  <si>
-    <t>76.1544</t>
+    <t>75.2034</t>
+  </si>
+  <si>
+    <t>86.7030</t>
   </si>
   <si>
     <t>26</t>
@@ -898,7 +898,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
-    <t>62.6244</t>
+    <t>88.6030</t>
   </si>
   <si>
     <t>28</t>
@@ -916,10 +916,10 @@
     <t>pedalboard-hw(3)</t>
   </si>
   <si>
-    <t>64.0194</t>
-  </si>
-  <si>
-    <t>89.5694</t>
+    <t>63.5410</t>
+  </si>
+  <si>
+    <t>89.9980</t>
   </si>
   <si>
     <t>29</t>
@@ -1027,10 +1027,10 @@
     <t>pedalboard-hw(5)</t>
   </si>
   <si>
-    <t>31.7744</t>
-  </si>
-  <si>
-    <t>78.3244</t>
+    <t>32.3744</t>
+  </si>
+  <si>
+    <t>78.3300</t>
   </si>
   <si>
     <t>35</t>
@@ -1147,10 +1147,10 @@
     <t>https://www.diodes.com/assets/Datasheets/AP255x.pdf</t>
   </si>
   <si>
-    <t>17.0944</t>
-  </si>
-  <si>
-    <t>103.9744</t>
+    <t>55.0870</t>
+  </si>
+  <si>
+    <t>79.1174</t>
   </si>
   <si>
     <t>3.6000</t>
@@ -1306,10 +1306,10 @@
     <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
-    <t>65.7444</t>
-  </si>
-  <si>
-    <t>80.6544</t>
+    <t>72.4560</t>
+  </si>
+  <si>
+    <t>91.7230</t>
   </si>
   <si>
     <t>10.8000</t>
@@ -2944,7 +2944,7 @@
         <v>98</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="S16" s="11" t="s">
         <v>40</v>
@@ -3228,7 +3228,7 @@
         <v>139</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="S20" s="11" t="s">
         <v>40</v>
@@ -3938,7 +3938,7 @@
         <v>248</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="S30" s="11" t="s">
         <v>40</v>
@@ -4151,7 +4151,7 @@
         <v>281</v>
       </c>
       <c r="R33" s="7" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="S33" s="7" t="s">
         <v>40</v>
@@ -4287,13 +4287,13 @@
         <v>63</v>
       </c>
       <c r="P35" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="Q35" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="R35" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>40</v>
@@ -4364,7 +4364,7 @@
         <v>299</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="S36" s="11" t="s">
         <v>40</v>
@@ -5429,7 +5429,7 @@
         <v>429</v>
       </c>
       <c r="R51" s="7" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="S51" s="7" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@06113cc3aee8fc2d82276c62f59bd8bfce252917 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -541,10 +541,10 @@
     <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
   </si>
   <si>
-    <t>127.8644</t>
-  </si>
-  <si>
-    <t>77.1844</t>
+    <t>128.2310</t>
+  </si>
+  <si>
+    <t>78.0252</t>
   </si>
   <si>
     <t>12.4000</t>
@@ -670,10 +670,10 @@
     <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
   </si>
   <si>
-    <t>160.4944</t>
-  </si>
-  <si>
-    <t>102.7844</t>
+    <t>157.6316</t>
+  </si>
+  <si>
+    <t>102.7958</t>
   </si>
   <si>
     <t>7.6000</t>
@@ -934,10 +934,10 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
-    <t>153.0944</t>
-  </si>
-  <si>
-    <t>100.1644</t>
+    <t>133.1920</t>
+  </si>
+  <si>
+    <t>107.2606</t>
   </si>
   <si>
     <t>30</t>
@@ -1510,10 +1510,10 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
-    <t>161.3944</t>
-  </si>
-  <si>
-    <t>100.5944</t>
+    <t>158.5316</t>
+  </si>
+  <si>
+    <t>100.6058</t>
   </si>
   <si>
     <t>no</t>
@@ -4435,7 +4435,7 @@
         <v>305</v>
       </c>
       <c r="R37" s="7" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="S37" s="7" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3d9719ddbe02320f05fc0cb8e2e94531d6b5ac03 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Positional/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Positional/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="572">
   <si>
     <t>Row</t>
   </si>
@@ -1169,9 +1169,6 @@
   </si>
   <si>
     <t>AP64351</t>
-  </si>
-  <si>
-    <t>CM4IO</t>
   </si>
   <si>
     <t>U6</t>
@@ -2323,7 +2320,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2348,13 +2345,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>503</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F2" s="3">
         <v>55</v>
@@ -2362,41 +2359,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>505</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>507</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>509</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2404,13 +2401,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>511</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F6" s="3">
         <v>128</v>
@@ -5196,16 +5193,16 @@
         <v>382</v>
       </c>
       <c r="D47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>385</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>386</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>107</v>
@@ -5220,10 +5217,10 @@
         <v>32</v>
       </c>
       <c r="L47" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="M47" s="8" t="s">
         <v>387</v>
-      </c>
-      <c r="M47" s="8" t="s">
-        <v>388</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>56</v>
@@ -5232,10 +5229,10 @@
         <v>64</v>
       </c>
       <c r="P47" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q47" s="7" t="s">
         <v>389</v>
-      </c>
-      <c r="Q47" s="7" t="s">
-        <v>390</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>75</v>
@@ -5250,33 +5247,33 @@
         <v>42</v>
       </c>
       <c r="V47" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="W47" s="7" t="s">
         <v>391</v>
-      </c>
-      <c r="W47" s="7" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="B48" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="C48" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="G48" s="11" t="s">
         <v>397</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>398</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>366</v>
@@ -5291,10 +5288,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="M48" s="12" t="s">
         <v>399</v>
-      </c>
-      <c r="M48" s="12" t="s">
-        <v>400</v>
       </c>
       <c r="N48" s="11" t="s">
         <v>35</v>
@@ -5303,10 +5300,10 @@
         <v>64</v>
       </c>
       <c r="P48" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q48" s="11" t="s">
         <v>401</v>
-      </c>
-      <c r="Q48" s="11" t="s">
-        <v>402</v>
       </c>
       <c r="R48" s="11" t="s">
         <v>39</v>
@@ -5329,28 +5326,28 @@
     </row>
     <row r="49" spans="1:23" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="F49" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="G49" s="7" t="s">
+      <c r="H49" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>409</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>23</v>
@@ -5362,10 +5359,10 @@
         <v>32</v>
       </c>
       <c r="L49" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="M49" s="8" t="s">
         <v>410</v>
-      </c>
-      <c r="M49" s="8" t="s">
-        <v>411</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>47</v>
@@ -5374,10 +5371,10 @@
         <v>64</v>
       </c>
       <c r="P49" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q49" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="Q49" s="7" t="s">
-        <v>413</v>
       </c>
       <c r="R49" s="7" t="s">
         <v>39</v>
@@ -5395,30 +5392,30 @@
         <v>153</v>
       </c>
       <c r="W49" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="F50" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>418</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>419</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>366</v>
@@ -5433,10 +5430,10 @@
         <v>32</v>
       </c>
       <c r="L50" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="M50" s="12" t="s">
         <v>420</v>
-      </c>
-      <c r="M50" s="12" t="s">
-        <v>421</v>
       </c>
       <c r="N50" s="11" t="s">
         <v>56</v>
@@ -5445,10 +5442,10 @@
         <v>64</v>
       </c>
       <c r="P50" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q50" s="11" t="s">
         <v>422</v>
-      </c>
-      <c r="Q50" s="11" t="s">
-        <v>423</v>
       </c>
       <c r="R50" s="11" t="s">
         <v>39</v>
@@ -5466,30 +5463,30 @@
         <v>100</v>
       </c>
       <c r="W50" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>104</v>
       </c>
       <c r="E51" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>426</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>428</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>107</v>
@@ -5504,10 +5501,10 @@
         <v>32</v>
       </c>
       <c r="L51" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="M51" s="8" t="s">
         <v>429</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>430</v>
       </c>
       <c r="N51" s="7" t="s">
         <v>35</v>
@@ -5516,10 +5513,10 @@
         <v>64</v>
       </c>
       <c r="P51" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q51" s="7" t="s">
         <v>431</v>
-      </c>
-      <c r="Q51" s="7" t="s">
-        <v>432</v>
       </c>
       <c r="R51" s="7" t="s">
         <v>50</v>
@@ -5534,36 +5531,36 @@
         <v>42</v>
       </c>
       <c r="V51" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="W51" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:23" ht="30" customHeight="1">
       <c r="A52" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="B52" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="C52" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="F52" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="G52" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>439</v>
-      </c>
       <c r="H52" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I52" s="9" t="s">
         <v>23</v>
@@ -5575,10 +5572,10 @@
         <v>32</v>
       </c>
       <c r="L52" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="M52" s="12" t="s">
         <v>440</v>
-      </c>
-      <c r="M52" s="12" t="s">
-        <v>441</v>
       </c>
       <c r="N52" s="11" t="s">
         <v>35</v>
@@ -5587,10 +5584,10 @@
         <v>64</v>
       </c>
       <c r="P52" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q52" s="11" t="s">
         <v>442</v>
-      </c>
-      <c r="Q52" s="11" t="s">
-        <v>443</v>
       </c>
       <c r="R52" s="11" t="s">
         <v>113</v>
@@ -5605,36 +5602,36 @@
         <v>42</v>
       </c>
       <c r="V52" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="W52" s="11" t="s">
         <v>444</v>
-      </c>
-      <c r="W52" s="11" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="53" spans="1:23" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="E53" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="G53" s="7" t="s">
+      <c r="H53" s="7" t="s">
         <v>451</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>452</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>23</v>
@@ -5646,10 +5643,10 @@
         <v>32</v>
       </c>
       <c r="L53" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="M53" s="8" t="s">
         <v>453</v>
-      </c>
-      <c r="M53" s="8" t="s">
-        <v>454</v>
       </c>
       <c r="N53" s="7" t="s">
         <v>47</v>
@@ -5658,10 +5655,10 @@
         <v>64</v>
       </c>
       <c r="P53" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q53" s="7" t="s">
         <v>455</v>
-      </c>
-      <c r="Q53" s="7" t="s">
-        <v>456</v>
       </c>
       <c r="R53" s="7" t="s">
         <v>39</v>
@@ -5676,36 +5673,36 @@
         <v>42</v>
       </c>
       <c r="V53" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="W53" s="7" t="s">
         <v>457</v>
-      </c>
-      <c r="W53" s="7" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:23" ht="30" customHeight="1">
       <c r="A54" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="C54" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="D54" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="E54" s="11" t="s">
+      <c r="F54" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="F54" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="G54" s="11" t="s">
+      <c r="H54" s="11" t="s">
         <v>463</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>464</v>
       </c>
       <c r="I54" s="9" t="s">
         <v>23</v>
@@ -5717,10 +5714,10 @@
         <v>32</v>
       </c>
       <c r="L54" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="M54" s="12" t="s">
         <v>465</v>
-      </c>
-      <c r="M54" s="12" t="s">
-        <v>466</v>
       </c>
       <c r="N54" s="11" t="s">
         <v>47</v>
@@ -5729,10 +5726,10 @@
         <v>64</v>
       </c>
       <c r="P54" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q54" s="11" t="s">
         <v>467</v>
-      </c>
-      <c r="Q54" s="11" t="s">
-        <v>468</v>
       </c>
       <c r="R54" s="11" t="s">
         <v>75</v>
@@ -5755,25 +5752,25 @@
     </row>
     <row r="55" spans="1:23" ht="30" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>104</v>
       </c>
       <c r="E55" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>472</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>473</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>107</v>
@@ -5788,10 +5785,10 @@
         <v>32</v>
       </c>
       <c r="L55" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="M55" s="8" t="s">
         <v>474</v>
-      </c>
-      <c r="M55" s="8" t="s">
-        <v>475</v>
       </c>
       <c r="N55" s="7" t="s">
         <v>35</v>
@@ -5800,10 +5797,10 @@
         <v>64</v>
       </c>
       <c r="P55" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q55" s="7" t="s">
         <v>476</v>
-      </c>
-      <c r="Q55" s="7" t="s">
-        <v>477</v>
       </c>
       <c r="R55" s="7" t="s">
         <v>50</v>
@@ -5818,33 +5815,33 @@
         <v>42</v>
       </c>
       <c r="V55" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="W55" s="7" t="s">
         <v>478</v>
-      </c>
-      <c r="W55" s="7" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="56" spans="1:23" ht="30" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>104</v>
       </c>
       <c r="E56" s="11" t="s">
+        <v>481</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>482</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>483</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>107</v>
@@ -5859,10 +5856,10 @@
         <v>32</v>
       </c>
       <c r="L56" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="M56" s="12" t="s">
         <v>484</v>
-      </c>
-      <c r="M56" s="12" t="s">
-        <v>485</v>
       </c>
       <c r="N56" s="11" t="s">
         <v>35</v>
@@ -5871,10 +5868,10 @@
         <v>64</v>
       </c>
       <c r="P56" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q56" s="11" t="s">
         <v>486</v>
-      </c>
-      <c r="Q56" s="11" t="s">
-        <v>487</v>
       </c>
       <c r="R56" s="11" t="s">
         <v>50</v>
@@ -5889,7 +5886,7 @@
         <v>42</v>
       </c>
       <c r="V56" s="11" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="W56" s="11" t="s">
         <v>379</v>
@@ -5897,28 +5894,28 @@
     </row>
     <row r="57" spans="1:23" ht="30" customHeight="1">
       <c r="A57" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="C57" s="7" t="s">
         <v>490</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>491</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E57" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="F57" s="7" t="s">
-        <v>491</v>
-      </c>
-      <c r="G57" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>493</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>494</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>23</v>
@@ -5930,10 +5927,10 @@
         <v>32</v>
       </c>
       <c r="L57" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="M57" s="8" t="s">
         <v>495</v>
-      </c>
-      <c r="M57" s="8" t="s">
-        <v>496</v>
       </c>
       <c r="N57" s="7" t="s">
         <v>47</v>
@@ -5942,10 +5939,10 @@
         <v>64</v>
       </c>
       <c r="P57" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q57" s="7" t="s">
         <v>497</v>
-      </c>
-      <c r="Q57" s="7" t="s">
-        <v>498</v>
       </c>
       <c r="R57" s="7" t="s">
         <v>75</v>
@@ -5960,10 +5957,10 @@
         <v>42</v>
       </c>
       <c r="V57" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="W57" s="7" t="s">
         <v>499</v>
-      </c>
-      <c r="W57" s="7" t="s">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -6014,7 +6011,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -6039,13 +6036,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="C2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>503</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F2" s="3">
         <v>55</v>
@@ -6053,41 +6050,41 @@
     </row>
     <row r="3" spans="1:23">
       <c r="C3" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>505</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="C4" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>507</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>515</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="C5" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>509</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -6095,13 +6092,13 @@
     </row>
     <row r="6" spans="1:23">
       <c r="C6" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>511</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F6" s="3">
         <v>128</v>
@@ -6186,19 +6183,19 @@
         <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>157</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>521</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>522</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>107</v>
@@ -6207,16 +6204,16 @@
         <v>23</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="8" t="s">
         <v>525</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>526</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>56</v>
@@ -6225,10 +6222,10 @@
         <v>64</v>
       </c>
       <c r="P9" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q9" s="7" t="s">
         <v>527</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>528</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>39</v>
@@ -6240,10 +6237,10 @@
         <v>187</v>
       </c>
       <c r="U9" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="V9" s="7" t="s">
         <v>529</v>
-      </c>
-      <c r="V9" s="7" t="s">
-        <v>530</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>219</v>
@@ -6257,19 +6254,19 @@
         <v>24</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>157</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>532</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>533</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>534</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>107</v>
@@ -6278,16 +6275,16 @@
         <v>31</v>
       </c>
       <c r="J10" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>524</v>
-      </c>
       <c r="L10" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="M10" s="12" t="s">
         <v>535</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>536</v>
       </c>
       <c r="N10" s="11" t="s">
         <v>35</v>
@@ -6296,10 +6293,10 @@
         <v>36</v>
       </c>
       <c r="P10" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q10" s="11" t="s">
         <v>537</v>
-      </c>
-      <c r="Q10" s="11" t="s">
-        <v>538</v>
       </c>
       <c r="R10" s="11" t="s">
         <v>39</v>
@@ -6311,13 +6308,13 @@
         <v>187</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="V10" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="W10" s="11" t="s">
         <v>539</v>
-      </c>
-      <c r="W10" s="11" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -6334,25 +6331,25 @@
         <v>157</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>543</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>544</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>523</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>524</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>120</v>
@@ -6367,10 +6364,10 @@
         <v>36</v>
       </c>
       <c r="P11" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>545</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>546</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>50</v>
@@ -6382,13 +6379,13 @@
         <v>187</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>371</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="30" customHeight="1">
@@ -6405,25 +6402,25 @@
         <v>157</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>159</v>
       </c>
       <c r="G12" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>549</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>550</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>523</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>524</v>
       </c>
       <c r="L12" s="11" t="s">
         <v>161</v>
@@ -6438,10 +6435,10 @@
         <v>36</v>
       </c>
       <c r="P12" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q12" s="11" t="s">
         <v>551</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>552</v>
       </c>
       <c r="R12" s="11" t="s">
         <v>113</v>
@@ -6453,13 +6450,13 @@
         <v>187</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="V12" s="11" t="s">
+        <v>552</v>
+      </c>
+      <c r="W12" s="11" t="s">
         <v>553</v>
-      </c>
-      <c r="W12" s="11" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -6476,10 +6473,10 @@
         <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>555</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>556</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>279</v>
@@ -6491,10 +6488,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>523</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>524</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>120</v>
@@ -6509,10 +6506,10 @@
         <v>64</v>
       </c>
       <c r="P13" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>557</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>558</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>113</v>
@@ -6524,7 +6521,7 @@
         <v>41</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>123</v>
@@ -6547,31 +6544,31 @@
         <v>352</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>559</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>561</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>562</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J14" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>524</v>
-      </c>
       <c r="L14" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>563</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>564</v>
       </c>
       <c r="N14" s="11" t="s">
         <v>35</v>
@@ -6580,10 +6577,10 @@
         <v>36</v>
       </c>
       <c r="P14" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q14" s="11" t="s">
         <v>565</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>566</v>
       </c>
       <c r="R14" s="11" t="s">
         <v>50</v>
@@ -6595,10 +6592,10 @@
         <v>41</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="W14" s="11" t="s">
         <v>371</v>
@@ -6627,27 +6624,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>